<commit_message>
refs #1 update README(Function)
</commit_message>
<xml_diff>
--- a/doc/めも_IOエキスパンダー自作.xlsx
+++ b/doc/めも_IOエキスパンダー自作.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="19200" windowHeight="12090"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="19200" windowHeight="12090" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="概要002" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="102">
   <si>
     <t>/START</t>
     <phoneticPr fontId="1"/>
@@ -41,10 +41,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>STOP</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>＜Write Sequence＞</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -54,17 +50,6 @@
   </si>
   <si>
     <t>＜Burst Write Sequence＞</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>＜Register Maps＞</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>REGISTER</t>
-  </si>
-  <si>
-    <t>ADDRESS</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -274,10 +259,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Analog Data1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Interrupt Flag</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -326,26 +307,75 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>I2C1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>0x11</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>SDA1</t>
+    <t>Default IO Value for INT</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>I2C Data1</t>
+    <t>Stop</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>0x12</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Default IO Value for INT</t>
+    <t>0x13</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>I2C1_WRITE</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>I2C Slave Address, Read Length</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>I2C1_READ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>＜Function Maps＞</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Function</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Address</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Type1: 1byte Read/Write</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Type2: nbyte Read/Write</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Analog Data(AD or DA)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Data</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ADR+R(8bit), LEN(8bit)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ADR+W(8bit), SDA(n bytes)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>I2C Slave Address, SDA</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -402,7 +432,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -584,13 +614,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -636,6 +703,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -645,10 +715,22 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6796,8 +6878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:BT32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:BS32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.125" defaultRowHeight="13.5"/>
@@ -11215,7 +11297,7 @@
   <dimension ref="A1:BJ41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P42" sqref="P42"/>
+      <selection activeCell="AE27" sqref="AE27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.25" defaultRowHeight="13.5"/>
@@ -11287,7 +11369,7 @@
     <row r="2" spans="1:62">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -11481,23 +11563,23 @@
     <row r="5" spans="1:62">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
@@ -11528,12 +11610,12 @@
       <c r="AQ5" s="1"/>
       <c r="AR5" s="1"/>
       <c r="AS5" s="1"/>
-      <c r="AT5" s="15" t="s">
-        <v>5</v>
+      <c r="AT5" s="16" t="s">
+        <v>86</v>
       </c>
-      <c r="AU5" s="15"/>
-      <c r="AV5" s="15"/>
-      <c r="AW5" s="15"/>
+      <c r="AU5" s="16"/>
+      <c r="AV5" s="16"/>
+      <c r="AW5" s="16"/>
       <c r="AX5" s="1"/>
       <c r="AY5" s="1"/>
       <c r="AZ5" s="1"/>
@@ -11551,19 +11633,19 @@
     <row r="6" spans="1:62">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
@@ -11594,10 +11676,10 @@
       <c r="AQ6" s="1"/>
       <c r="AR6" s="1"/>
       <c r="AS6" s="1"/>
-      <c r="AT6" s="15"/>
-      <c r="AU6" s="15"/>
-      <c r="AV6" s="15"/>
-      <c r="AW6" s="15"/>
+      <c r="AT6" s="16"/>
+      <c r="AU6" s="16"/>
+      <c r="AV6" s="16"/>
+      <c r="AW6" s="16"/>
       <c r="AX6" s="1"/>
       <c r="AY6" s="1"/>
       <c r="AZ6" s="1"/>
@@ -11679,14 +11761,14 @@
     <row r="8" spans="1:62" ht="13.5" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -11710,14 +11792,14 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
       <c r="AE8" s="1"/>
-      <c r="AF8" s="17" t="s">
+      <c r="AF8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="AG8" s="17"/>
-      <c r="AH8" s="17"/>
-      <c r="AI8" s="17"/>
-      <c r="AJ8" s="17"/>
-      <c r="AK8" s="17"/>
+      <c r="AG8" s="18"/>
+      <c r="AH8" s="18"/>
+      <c r="AI8" s="18"/>
+      <c r="AJ8" s="18"/>
+      <c r="AK8" s="18"/>
       <c r="AL8" s="1"/>
       <c r="AM8" s="1"/>
       <c r="AN8" s="1"/>
@@ -11747,12 +11829,12 @@
     <row r="9" spans="1:62" ht="13.5" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -11776,12 +11858,12 @@
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
       <c r="AE9" s="1"/>
-      <c r="AF9" s="17"/>
-      <c r="AG9" s="17"/>
-      <c r="AH9" s="17"/>
-      <c r="AI9" s="17"/>
-      <c r="AJ9" s="17"/>
-      <c r="AK9" s="17"/>
+      <c r="AF9" s="18"/>
+      <c r="AG9" s="18"/>
+      <c r="AH9" s="18"/>
+      <c r="AI9" s="18"/>
+      <c r="AJ9" s="18"/>
+      <c r="AK9" s="18"/>
       <c r="AL9" s="1"/>
       <c r="AM9" s="1"/>
       <c r="AN9" s="1"/>
@@ -11875,14 +11957,14 @@
     <row r="11" spans="1:62">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -11909,14 +11991,14 @@
       <c r="AF11" s="1"/>
       <c r="AG11" s="1"/>
       <c r="AH11" s="1"/>
-      <c r="AI11" s="17" t="s">
+      <c r="AI11" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="AJ11" s="17"/>
-      <c r="AK11" s="17"/>
-      <c r="AL11" s="17"/>
-      <c r="AM11" s="17"/>
-      <c r="AN11" s="17"/>
+      <c r="AJ11" s="18"/>
+      <c r="AK11" s="18"/>
+      <c r="AL11" s="18"/>
+      <c r="AM11" s="18"/>
+      <c r="AN11" s="18"/>
       <c r="AO11" s="1"/>
       <c r="AP11" s="1"/>
       <c r="AQ11" s="1"/>
@@ -11943,12 +12025,12 @@
     <row r="12" spans="1:62">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -11975,12 +12057,12 @@
       <c r="AF12" s="1"/>
       <c r="AG12" s="1"/>
       <c r="AH12" s="1"/>
-      <c r="AI12" s="17"/>
-      <c r="AJ12" s="17"/>
-      <c r="AK12" s="17"/>
-      <c r="AL12" s="17"/>
-      <c r="AM12" s="17"/>
-      <c r="AN12" s="17"/>
+      <c r="AI12" s="18"/>
+      <c r="AJ12" s="18"/>
+      <c r="AK12" s="18"/>
+      <c r="AL12" s="18"/>
+      <c r="AM12" s="18"/>
+      <c r="AN12" s="18"/>
       <c r="AO12" s="1"/>
       <c r="AP12" s="1"/>
       <c r="AQ12" s="1"/>
@@ -12135,7 +12217,7 @@
     <row r="15" spans="1:62">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -12329,23 +12411,23 @@
     <row r="18" spans="1:62">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
-      <c r="L18" s="15" t="s">
+      <c r="L18" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
@@ -12383,12 +12465,12 @@
       <c r="AX18" s="1"/>
       <c r="AY18" s="1"/>
       <c r="AZ18" s="1"/>
-      <c r="BA18" s="15" t="s">
-        <v>5</v>
+      <c r="BA18" s="16" t="s">
+        <v>86</v>
       </c>
-      <c r="BB18" s="15"/>
-      <c r="BC18" s="15"/>
-      <c r="BD18" s="15"/>
+      <c r="BB18" s="16"/>
+      <c r="BC18" s="16"/>
+      <c r="BD18" s="16"/>
       <c r="BE18" s="1"/>
       <c r="BF18" s="1"/>
       <c r="BG18" s="1"/>
@@ -12399,19 +12481,19 @@
     <row r="19" spans="1:62">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
@@ -12449,10 +12531,10 @@
       <c r="AX19" s="1"/>
       <c r="AY19" s="1"/>
       <c r="AZ19" s="1"/>
-      <c r="BA19" s="15"/>
-      <c r="BB19" s="15"/>
-      <c r="BC19" s="15"/>
-      <c r="BD19" s="15"/>
+      <c r="BA19" s="16"/>
+      <c r="BB19" s="16"/>
+      <c r="BC19" s="16"/>
+      <c r="BD19" s="16"/>
       <c r="BE19" s="1"/>
       <c r="BF19" s="1"/>
       <c r="BG19" s="1"/>
@@ -12527,14 +12609,14 @@
     <row r="21" spans="1:62">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -12572,14 +12654,14 @@
       <c r="AQ21" s="1"/>
       <c r="AR21" s="1"/>
       <c r="AS21" s="1"/>
-      <c r="AT21" s="17" t="s">
+      <c r="AT21" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="AU21" s="17"/>
-      <c r="AV21" s="17"/>
-      <c r="AW21" s="17"/>
-      <c r="AX21" s="17"/>
-      <c r="AY21" s="17"/>
+      <c r="AU21" s="18"/>
+      <c r="AV21" s="18"/>
+      <c r="AW21" s="18"/>
+      <c r="AX21" s="18"/>
+      <c r="AY21" s="18"/>
       <c r="AZ21" s="1"/>
       <c r="BA21" s="1"/>
       <c r="BB21" s="1"/>
@@ -12595,12 +12677,12 @@
     <row r="22" spans="1:62">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -12638,12 +12720,12 @@
       <c r="AQ22" s="1"/>
       <c r="AR22" s="1"/>
       <c r="AS22" s="1"/>
-      <c r="AT22" s="17"/>
-      <c r="AU22" s="17"/>
-      <c r="AV22" s="17"/>
-      <c r="AW22" s="17"/>
-      <c r="AX22" s="17"/>
-      <c r="AY22" s="17"/>
+      <c r="AT22" s="18"/>
+      <c r="AU22" s="18"/>
+      <c r="AV22" s="18"/>
+      <c r="AW22" s="18"/>
+      <c r="AX22" s="18"/>
+      <c r="AY22" s="18"/>
       <c r="AZ22" s="1"/>
       <c r="BA22" s="1"/>
       <c r="BB22" s="1"/>
@@ -12723,14 +12805,14 @@
     <row r="24" spans="1:62">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -12768,14 +12850,14 @@
       <c r="AQ24" s="1"/>
       <c r="AR24" s="1"/>
       <c r="AS24" s="1"/>
-      <c r="AT24" s="17" t="s">
+      <c r="AT24" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="AU24" s="17"/>
-      <c r="AV24" s="17"/>
-      <c r="AW24" s="17"/>
-      <c r="AX24" s="17"/>
-      <c r="AY24" s="17"/>
+      <c r="AU24" s="18"/>
+      <c r="AV24" s="18"/>
+      <c r="AW24" s="18"/>
+      <c r="AX24" s="18"/>
+      <c r="AY24" s="18"/>
       <c r="AZ24" s="1"/>
       <c r="BA24" s="1"/>
       <c r="BB24" s="1"/>
@@ -12791,12 +12873,12 @@
     <row r="25" spans="1:62">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -12834,12 +12916,12 @@
       <c r="AQ25" s="1"/>
       <c r="AR25" s="1"/>
       <c r="AS25" s="1"/>
-      <c r="AT25" s="17"/>
-      <c r="AU25" s="17"/>
-      <c r="AV25" s="17"/>
-      <c r="AW25" s="17"/>
-      <c r="AX25" s="17"/>
-      <c r="AY25" s="17"/>
+      <c r="AT25" s="18"/>
+      <c r="AU25" s="18"/>
+      <c r="AV25" s="18"/>
+      <c r="AW25" s="18"/>
+      <c r="AX25" s="18"/>
+      <c r="AY25" s="18"/>
       <c r="AZ25" s="1"/>
       <c r="BA25" s="1"/>
       <c r="BB25" s="1"/>
@@ -12983,7 +13065,7 @@
     <row r="28" spans="1:62">
       <c r="A28" s="1"/>
       <c r="B28" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -13177,23 +13259,23 @@
     <row r="31" spans="1:62">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
-      <c r="L31" s="15" t="s">
+      <c r="L31" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="16"/>
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
@@ -13228,12 +13310,12 @@
       <c r="AU31" s="1"/>
       <c r="AV31" s="1"/>
       <c r="AW31" s="1"/>
-      <c r="AX31" s="15" t="s">
-        <v>5</v>
+      <c r="AX31" s="16" t="s">
+        <v>86</v>
       </c>
-      <c r="AY31" s="15"/>
-      <c r="AZ31" s="15"/>
-      <c r="BA31" s="15"/>
+      <c r="AY31" s="16"/>
+      <c r="AZ31" s="16"/>
+      <c r="BA31" s="16"/>
       <c r="BB31" s="1"/>
       <c r="BC31" s="1"/>
       <c r="BD31" s="1"/>
@@ -13247,19 +13329,19 @@
     <row r="32" spans="1:62">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
-      <c r="O32" s="15"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="16"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="16"/>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
@@ -13294,10 +13376,10 @@
       <c r="AU32" s="1"/>
       <c r="AV32" s="1"/>
       <c r="AW32" s="1"/>
-      <c r="AX32" s="15"/>
-      <c r="AY32" s="15"/>
-      <c r="AZ32" s="15"/>
-      <c r="BA32" s="15"/>
+      <c r="AX32" s="16"/>
+      <c r="AY32" s="16"/>
+      <c r="AZ32" s="16"/>
+      <c r="BA32" s="16"/>
       <c r="BB32" s="1"/>
       <c r="BC32" s="1"/>
       <c r="BD32" s="1"/>
@@ -13375,14 +13457,14 @@
     <row r="34" spans="1:62">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
@@ -13416,14 +13498,14 @@
       <c r="AM34" s="1"/>
       <c r="AN34" s="1"/>
       <c r="AO34" s="1"/>
-      <c r="AP34" s="17" t="s">
+      <c r="AP34" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="AQ34" s="17"/>
-      <c r="AR34" s="17"/>
-      <c r="AS34" s="17"/>
-      <c r="AT34" s="17"/>
-      <c r="AU34" s="17"/>
+      <c r="AQ34" s="18"/>
+      <c r="AR34" s="18"/>
+      <c r="AS34" s="18"/>
+      <c r="AT34" s="18"/>
+      <c r="AU34" s="18"/>
       <c r="AV34" s="1"/>
       <c r="AW34" s="1"/>
       <c r="AX34" s="1"/>
@@ -13443,12 +13525,12 @@
     <row r="35" spans="1:62">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -13482,12 +13564,12 @@
       <c r="AM35" s="1"/>
       <c r="AN35" s="1"/>
       <c r="AO35" s="1"/>
-      <c r="AP35" s="17"/>
-      <c r="AQ35" s="17"/>
-      <c r="AR35" s="17"/>
-      <c r="AS35" s="17"/>
-      <c r="AT35" s="17"/>
-      <c r="AU35" s="17"/>
+      <c r="AP35" s="18"/>
+      <c r="AQ35" s="18"/>
+      <c r="AR35" s="18"/>
+      <c r="AS35" s="18"/>
+      <c r="AT35" s="18"/>
+      <c r="AU35" s="18"/>
       <c r="AV35" s="1"/>
       <c r="AW35" s="1"/>
       <c r="AX35" s="1"/>
@@ -13571,14 +13653,14 @@
     <row r="37" spans="1:62">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
-      <c r="C37" s="16" t="s">
+      <c r="C37" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="16"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
@@ -13612,14 +13694,14 @@
       <c r="AM37" s="1"/>
       <c r="AN37" s="1"/>
       <c r="AO37" s="1"/>
-      <c r="AP37" s="17" t="s">
+      <c r="AP37" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="AQ37" s="17"/>
-      <c r="AR37" s="17"/>
-      <c r="AS37" s="17"/>
-      <c r="AT37" s="17"/>
-      <c r="AU37" s="17"/>
+      <c r="AQ37" s="18"/>
+      <c r="AR37" s="18"/>
+      <c r="AS37" s="18"/>
+      <c r="AT37" s="18"/>
+      <c r="AU37" s="18"/>
       <c r="AV37" s="1"/>
       <c r="AW37" s="1"/>
       <c r="AX37" s="1"/>
@@ -13639,12 +13721,12 @@
     <row r="38" spans="1:62">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
@@ -13678,12 +13760,12 @@
       <c r="AM38" s="1"/>
       <c r="AN38" s="1"/>
       <c r="AO38" s="1"/>
-      <c r="AP38" s="17"/>
-      <c r="AQ38" s="17"/>
-      <c r="AR38" s="17"/>
-      <c r="AS38" s="17"/>
-      <c r="AT38" s="17"/>
-      <c r="AU38" s="17"/>
+      <c r="AP38" s="18"/>
+      <c r="AQ38" s="18"/>
+      <c r="AR38" s="18"/>
+      <c r="AS38" s="18"/>
+      <c r="AT38" s="18"/>
+      <c r="AU38" s="18"/>
       <c r="AV38" s="1"/>
       <c r="AW38" s="1"/>
       <c r="AX38" s="1"/>
@@ -13925,10 +14007,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:O15"/>
+  <dimension ref="B2:O20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:O15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -13938,7 +14020,7 @@
     <col min="4" max="4" width="11.625" customWidth="1"/>
     <col min="5" max="5" width="11.5" customWidth="1"/>
     <col min="6" max="6" width="9.375" customWidth="1"/>
-    <col min="14" max="14" width="22.375" customWidth="1"/>
+    <col min="14" max="14" width="31.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:15">
@@ -13960,7 +14042,7 @@
     <row r="3" spans="2:15">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>92</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -13975,7 +14057,7 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="2:15" ht="14.25" thickBot="1">
+    <row r="4" spans="2:15">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -13994,114 +14076,94 @@
     <row r="5" spans="2:15" ht="14.25" thickBot="1">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="2:15" ht="14.25" thickBot="1">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>11</v>
+      <c r="M6" s="4" t="s">
+        <v>9</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="O5" s="1"/>
-    </row>
-    <row r="6" spans="2:15">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>78</v>
+      <c r="N6" s="5" t="s">
+        <v>68</v>
       </c>
       <c r="O6" s="1"/>
     </row>
     <row r="7" spans="2:15">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="9" t="s">
-        <v>22</v>
+      <c r="D7" s="6" t="s">
+        <v>16</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>23</v>
+      <c r="E7" s="7" t="s">
+        <v>17</v>
       </c>
-      <c r="F7" s="10" t="s">
-        <v>24</v>
+      <c r="F7" s="7" t="s">
+        <v>32</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>26</v>
+      <c r="G7" s="7" t="s">
+        <v>33</v>
       </c>
-      <c r="H7" s="10" t="s">
-        <v>27</v>
+      <c r="H7" s="7" t="s">
+        <v>34</v>
       </c>
-      <c r="I7" s="10" t="s">
-        <v>28</v>
+      <c r="I7" s="7" t="s">
+        <v>35</v>
       </c>
-      <c r="J7" s="10" t="s">
-        <v>29</v>
+      <c r="J7" s="7" t="s">
+        <v>36</v>
       </c>
-      <c r="K7" s="10" t="s">
-        <v>30</v>
+      <c r="K7" s="7" t="s">
+        <v>37</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="L7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="M7" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="N7" s="11" t="s">
-        <v>77</v>
+      <c r="N7" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="O7" s="1"/>
     </row>
@@ -14109,37 +14171,37 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="9" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="N8" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="O8" s="1"/>
     </row>
@@ -14147,37 +14209,37 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="9" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="M9" s="10" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="N9" s="11" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="O9" s="1"/>
     </row>
@@ -14185,37 +14247,37 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="9" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="M10" s="10" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="N10" s="11" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="O10" s="1"/>
     </row>
@@ -14223,124 +14285,246 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="9" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="M11" s="10" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="N11" s="11" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="2:15">
+    <row r="12" spans="2:15" ht="14.25" thickBot="1">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="9" t="s">
-        <v>73</v>
+      <c r="D12" s="12" t="s">
+        <v>66</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>90</v>
+      <c r="E12" s="13" t="s">
+        <v>74</v>
       </c>
-      <c r="F12" s="18" t="s">
-        <v>88</v>
+      <c r="F12" s="13" t="s">
+        <v>76</v>
       </c>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="11" t="s">
-        <v>74</v>
+      <c r="G12" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="M12" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="N12" s="14" t="s">
+        <v>67</v>
       </c>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="2:15" ht="14.25" thickBot="1">
+    <row r="13" spans="2:15">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+    </row>
+    <row r="14" spans="2:15" ht="14.25" thickBot="1">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+    </row>
+    <row r="15" spans="2:15" ht="14.25" thickBot="1">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="2:15">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22"/>
+      <c r="N16" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="2:15">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="E13" s="13" t="s">
-        <v>93</v>
+      <c r="E17" s="10" t="s">
+        <v>87</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="F17" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="2:15" ht="14.25" thickBot="1">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="14" t="s">
-        <v>92</v>
+      <c r="E18" s="13" t="s">
+        <v>88</v>
       </c>
-      <c r="O13" s="1"/>
+      <c r="F18" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="O18" s="1"/>
     </row>
-    <row r="14" spans="2:15">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
+    <row r="19" spans="2:15">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
     </row>
-    <row r="15" spans="2:15">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
+    <row r="20" spans="2:15">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="F12:M12"/>
-    <mergeCell ref="F13:M13"/>
+  <mergeCells count="4">
+    <mergeCell ref="F15:M15"/>
+    <mergeCell ref="F16:M16"/>
+    <mergeCell ref="F18:M18"/>
+    <mergeCell ref="F17:M17"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix Function Maps. add uart command handling code (i2c only).
</commit_message>
<xml_diff>
--- a/doc/めも_IOエキスパンダー自作.xlsx
+++ b/doc/めも_IOエキスパンダー自作.xlsx
@@ -323,10 +323,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>I2C Slave Address, Read Length</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>I2C1_READ</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -355,19 +351,23 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ADR+R(8bit), LEN(8bit)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ADR+W(8bit), SDA(n bytes)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>I2C Slave Address, SDA</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>FuncNo.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ADR+R(8bit)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>I2C Slave Address</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ADR+W(8bit), SDA(n bytes)</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -11356,16 +11356,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AM5:AP6"/>
+    <mergeCell ref="AR18:AU19"/>
+    <mergeCell ref="C21:H22"/>
+    <mergeCell ref="C24:H25"/>
     <mergeCell ref="C8:H9"/>
     <mergeCell ref="C5:H6"/>
     <mergeCell ref="C11:H12"/>
     <mergeCell ref="M5:P6"/>
     <mergeCell ref="C18:H19"/>
     <mergeCell ref="M18:P19"/>
-    <mergeCell ref="AM5:AP6"/>
-    <mergeCell ref="AR18:AU19"/>
-    <mergeCell ref="C21:H22"/>
-    <mergeCell ref="C24:H25"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11379,7 +11379,7 @@
   <dimension ref="B2:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -11411,7 +11411,7 @@
     <row r="3" spans="2:15">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -11446,7 +11446,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -11464,10 +11464,10 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>6</v>
@@ -11746,7 +11746,7 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
@@ -11764,13 +11764,13 @@
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>
@@ -11804,7 +11804,7 @@
       <c r="L16" s="21"/>
       <c r="M16" s="21"/>
       <c r="N16" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O16" s="1"/>
     </row>
@@ -11818,7 +11818,7 @@
         <v>85</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="G17" s="23"/>
       <c r="H17" s="23"/>
@@ -11828,7 +11828,7 @@
       <c r="L17" s="23"/>
       <c r="M17" s="23"/>
       <c r="N17" s="11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="O17" s="1"/>
     </row>
@@ -11836,13 +11836,13 @@
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>86</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="22"/>
@@ -11852,7 +11852,7 @@
       <c r="L18" s="22"/>
       <c r="M18" s="22"/>
       <c r="N18" s="14" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="O18" s="1"/>
     </row>

</xml_diff>

<commit_message>
update README & add examples.
</commit_message>
<xml_diff>
--- a/doc/めも_IOエキスパンダー自作.xlsx
+++ b/doc/めも_IOエキスパンダー自作.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="19200" windowHeight="12090" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="19200" windowHeight="12090"/>
   </bookViews>
   <sheets>
     <sheet name="ピン配置" sheetId="6" r:id="rId1"/>
@@ -894,7 +894,7 @@
       <xdr:row>23</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1028700" cy="264560"/>
+    <xdr:ext cx="1276350" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="48" name="テキスト ボックス 47"/>
@@ -903,7 +903,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5676900" y="3990975"/>
-          <a:ext cx="1028700" cy="264560"/>
+          <a:ext cx="1276350" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -943,7 +943,7 @@
               <a:latin typeface="メイリオ" pitchFamily="50" charset="-128"/>
               <a:ea typeface="メイリオ" pitchFamily="50" charset="-128"/>
             </a:rPr>
-            <a:t>Digital0</a:t>
+            <a:t>Digital0(INT0)</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050" b="1">
             <a:latin typeface="メイリオ" pitchFamily="50" charset="-128"/>
@@ -1490,6 +1490,46 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>82</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 1" descr="「arduino nano pinout」の画像検索結果"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7953375" y="1543050"/>
+          <a:ext cx="5324475" cy="5324475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6926,8 +6966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="F1:AW41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AW8" sqref="AW8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="AR28" sqref="AR28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.125" defaultRowHeight="13.5"/>
@@ -17419,8 +17459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:O19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
change command sequence(passing build only)
</commit_message>
<xml_diff>
--- a/doc/めも_IOエキスパンダー自作.xlsx
+++ b/doc/めも_IOエキスパンダー自作.xlsx
@@ -4,21 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="19200" windowHeight="12090"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="19200" windowHeight="12090" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ピン配置" sheetId="6" r:id="rId1"/>
     <sheet name="概要002" sheetId="4" r:id="rId2"/>
     <sheet name="概要001" sheetId="1" r:id="rId3"/>
-    <sheet name="通信シーケンス" sheetId="3" r:id="rId4"/>
-    <sheet name="機能一覧" sheetId="5" r:id="rId5"/>
+    <sheet name="通信シーケンス002" sheetId="7" r:id="rId4"/>
+    <sheet name="通信シーケンス001" sheetId="3" r:id="rId5"/>
+    <sheet name="機能一覧" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="100">
   <si>
     <t>/START</t>
     <phoneticPr fontId="1"/>
@@ -345,12 +346,69 @@
   <si>
     <t>Default IO Value for INT</t>
   </si>
+  <si>
+    <t>・</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>※I2Cでも使用できるような体系にする</t>
+    <rPh sb="6" eb="8">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>タイケイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>参考（Ｉ２Ｃ）</t>
+    <rPh sb="0" eb="2">
+      <t>サンコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>HostからのDATA内に0x10(=DLE)を含む場合は</t>
+    <rPh sb="11" eb="12">
+      <t>ナイ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>フク</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>バアイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x10-&gt;0x1010と変換する（エスケープシーケンスの要領）</t>
+    <rPh sb="13" eb="15">
+      <t>ヘンカン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Start by Host</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Sequence Version002</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Sequence Version001</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>replace 0x10(DLE) by 0x10+0x10 in Host Data</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,6 +440,15 @@
       <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -627,7 +694,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -679,11 +746,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -5032,13 +5102,1364 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>52</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="直線コネクタ 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371600" y="1028700"/>
+          <a:ext cx="7543800" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>52</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="直線コネクタ 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371600" y="1543050"/>
+          <a:ext cx="7543800" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="正方形/長方形 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1885950" y="685800"/>
+          <a:ext cx="1200150" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>DLE+STX</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1000">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="正方形/長方形 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3771900" y="685800"/>
+          <a:ext cx="171450" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>W</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="正方形/長方形 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3943350" y="1200150"/>
+          <a:ext cx="857250" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Size</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="正方形/長方形 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6343650" y="1200150"/>
+          <a:ext cx="685800" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ACK</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="正方形/長方形 10"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4800600" y="1200150"/>
+          <a:ext cx="1371600" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" b="0" i="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>DATA(n bytes)</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="0" i="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="直線コネクタ 14"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371600" y="2743200"/>
+          <a:ext cx="8058150" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="直線コネクタ 15"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371600" y="3257550"/>
+          <a:ext cx="8058150" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="正方形/長方形 18"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3771900" y="2400300"/>
+          <a:ext cx="171450" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>R</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="正方形/長方形 19"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4972050" y="2914650"/>
+          <a:ext cx="685800" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ACK</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="正方形/長方形 23"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1885950" y="2400300"/>
+          <a:ext cx="1200150" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>DLE+STX</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1000">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="正方形/長方形 24"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3943350" y="3429000"/>
+          <a:ext cx="857250" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Size</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="正方形/長方形 25"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5657850" y="2914650"/>
+          <a:ext cx="1371600" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>DATA(n bytes)</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="正方形/長方形 26"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3086100" y="685800"/>
+          <a:ext cx="685800" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>FuncNo.</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="正方形/長方形 27"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3086100" y="2400300"/>
+          <a:ext cx="685800" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>FuncNo.</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="正方形/長方形 28"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7200900" y="685800"/>
+          <a:ext cx="1200150" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>DLE+ETX</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="正方形/長方形 31"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7886700" y="2400300"/>
+          <a:ext cx="1200150" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>DLE+ETX</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>171449</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>30808</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1025" name="Picture 1" descr="https://lh3.googleusercontent.com/proxy/eKgKX3nZCR8lNvfYMdtd3Sp7UOr1KB-9Co1VYmIsSfFTsMc6Vp_XaFXAiJI7cOOF-TXm45sRSFH8MQxB45oYAkZ0Cr4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1885949" y="4800600"/>
+          <a:ext cx="6515101" cy="2774008"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="正方形/長方形 41"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7200900" y="2400300"/>
+          <a:ext cx="685800" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ACK</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -5081,13 +6502,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>44</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -5130,13 +6551,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>44</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -5179,13 +6600,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -5228,13 +6649,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -5277,13 +6698,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5351,13 +6772,13 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5425,13 +6846,13 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5499,13 +6920,13 @@
     <xdr:from>
       <xdr:col>37</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>41</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5573,13 +6994,13 @@
     <xdr:from>
       <xdr:col>28</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>36</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5647,13 +7068,13 @@
     <xdr:from>
       <xdr:col>37</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -5696,13 +7117,13 @@
     <xdr:from>
       <xdr:col>38</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>44</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -5745,13 +7166,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -5794,13 +7215,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>49</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -5843,13 +7264,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>49</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -5892,13 +7313,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -5941,13 +7362,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -5990,13 +7411,13 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6064,13 +7485,13 @@
     <xdr:from>
       <xdr:col>29</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6138,13 +7559,13 @@
     <xdr:from>
       <xdr:col>43</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>47</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6212,13 +7633,13 @@
     <xdr:from>
       <xdr:col>42</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>43</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -6261,13 +7682,13 @@
     <xdr:from>
       <xdr:col>43</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>49</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -6310,13 +7731,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6384,13 +7805,13 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6458,13 +7879,13 @@
     <xdr:from>
       <xdr:col>33</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>41</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6532,13 +7953,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6606,13 +8027,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6966,7 +8387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="F1:AW41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="AR28" sqref="AR28"/>
     </sheetView>
   </sheetViews>
@@ -15513,89 +16934,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BP27"/>
+  <dimension ref="A1:BP33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AJ34" sqref="AJ34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:BP22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.25" defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:68">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1"/>
-      <c r="AD1" s="1"/>
-      <c r="AE1" s="1"/>
-      <c r="AF1" s="1"/>
-      <c r="AG1" s="1"/>
-      <c r="AH1" s="1"/>
-      <c r="AI1" s="1"/>
-      <c r="AJ1" s="1"/>
-      <c r="AK1" s="1"/>
-      <c r="AL1" s="1"/>
-      <c r="AM1" s="1"/>
-      <c r="AN1" s="1"/>
-      <c r="AO1" s="1"/>
-      <c r="AP1" s="1"/>
-      <c r="AQ1" s="1"/>
-      <c r="AR1" s="1"/>
-      <c r="AS1" s="1"/>
-      <c r="AT1" s="1"/>
-      <c r="AU1" s="1"/>
-      <c r="AV1" s="1"/>
-      <c r="AW1" s="1"/>
-      <c r="AX1" s="1"/>
-      <c r="AY1" s="1"/>
-      <c r="AZ1" s="1"/>
-      <c r="BA1" s="1"/>
-      <c r="BB1" s="1"/>
-      <c r="BC1" s="1"/>
-      <c r="BD1" s="1"/>
-      <c r="BE1" s="1"/>
-      <c r="BF1" s="1"/>
-      <c r="BG1" s="1"/>
-      <c r="BH1" s="1"/>
-      <c r="BI1" s="1"/>
-      <c r="BJ1" s="1"/>
-      <c r="BK1" s="1"/>
-      <c r="BL1" s="1"/>
-      <c r="BM1" s="1"/>
-      <c r="BN1" s="1"/>
-      <c r="BO1" s="1"/>
-      <c r="BP1" s="1"/>
+      <c r="A1" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="2" spans="1:68">
       <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -15665,7 +17019,9 @@
     </row>
     <row r="3" spans="1:68">
       <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -15806,24 +17162,20 @@
     <row r="5" spans="1:68">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
@@ -15846,12 +17198,10 @@
       <c r="AJ5" s="1"/>
       <c r="AK5" s="1"/>
       <c r="AL5" s="1"/>
-      <c r="AM5" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="AN5" s="17"/>
-      <c r="AO5" s="17"/>
-      <c r="AP5" s="17"/>
+      <c r="AM5" s="1"/>
+      <c r="AN5" s="1"/>
+      <c r="AO5" s="1"/>
+      <c r="AP5" s="1"/>
       <c r="AQ5" s="1"/>
       <c r="AR5" s="1"/>
       <c r="AS5" s="1"/>
@@ -15879,23 +17229,25 @@
       <c r="BO5" s="1"/>
       <c r="BP5" s="1"/>
     </row>
-    <row r="6" spans="1:68">
+    <row r="6" spans="1:68" ht="13.5" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
+      <c r="C6" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
@@ -15918,10 +17270,10 @@
       <c r="AJ6" s="1"/>
       <c r="AK6" s="1"/>
       <c r="AL6" s="1"/>
-      <c r="AM6" s="17"/>
-      <c r="AN6" s="17"/>
-      <c r="AO6" s="17"/>
-      <c r="AP6" s="17"/>
+      <c r="AM6" s="1"/>
+      <c r="AN6" s="1"/>
+      <c r="AO6" s="1"/>
+      <c r="AP6" s="1"/>
       <c r="AQ6" s="1"/>
       <c r="AR6" s="1"/>
       <c r="AS6" s="1"/>
@@ -15949,15 +17301,15 @@
       <c r="BO6" s="1"/>
       <c r="BP6" s="1"/>
     </row>
-    <row r="7" spans="1:68">
+    <row r="7" spans="1:68" ht="13.5" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -16019,17 +17371,15 @@
       <c r="BO7" s="1"/>
       <c r="BP7" s="1"/>
     </row>
-    <row r="8" spans="1:68" ht="13.5" customHeight="1">
+    <row r="8" spans="1:68">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -16094,7 +17444,9 @@
     <row r="9" spans="1:68" ht="13.5" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="18"/>
+      <c r="C9" s="18" t="s">
+        <v>2</v>
+      </c>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
@@ -16161,15 +17513,15 @@
       <c r="BO9" s="1"/>
       <c r="BP9" s="1"/>
     </row>
-    <row r="10" spans="1:68">
+    <row r="10" spans="1:68" ht="13.5" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -16231,17 +17583,15 @@
       <c r="BO10" s="1"/>
       <c r="BP10" s="1"/>
     </row>
-    <row r="11" spans="1:68" ht="13.5" customHeight="1">
+    <row r="11" spans="1:68">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -16303,15 +17653,15 @@
       <c r="BO11" s="1"/>
       <c r="BP11" s="1"/>
     </row>
-    <row r="12" spans="1:68" ht="13.5" customHeight="1">
+    <row r="12" spans="1:68">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -16375,7 +17725,9 @@
     </row>
     <row r="13" spans="1:68">
       <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="B13" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -16515,9 +17867,1558 @@
     </row>
     <row r="15" spans="1:68">
       <c r="A15" s="1"/>
-      <c r="B15" s="2" t="s">
-        <v>5</v>
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
+      <c r="AD15" s="1"/>
+      <c r="AE15" s="1"/>
+      <c r="AF15" s="1"/>
+      <c r="AG15" s="1"/>
+      <c r="AH15" s="1"/>
+      <c r="AI15" s="1"/>
+      <c r="AJ15" s="1"/>
+      <c r="AK15" s="1"/>
+      <c r="AL15" s="1"/>
+      <c r="AM15" s="1"/>
+      <c r="AN15" s="1"/>
+      <c r="AO15" s="1"/>
+      <c r="AP15" s="1"/>
+      <c r="AQ15" s="1"/>
+      <c r="AR15" s="1"/>
+      <c r="AS15" s="1"/>
+      <c r="AT15" s="1"/>
+      <c r="AU15" s="1"/>
+      <c r="AV15" s="1"/>
+      <c r="AW15" s="1"/>
+      <c r="AX15" s="1"/>
+      <c r="AY15" s="1"/>
+      <c r="AZ15" s="1"/>
+      <c r="BA15" s="1"/>
+      <c r="BB15" s="1"/>
+      <c r="BC15" s="1"/>
+      <c r="BD15" s="1"/>
+      <c r="BE15" s="1"/>
+      <c r="BF15" s="1"/>
+      <c r="BG15" s="1"/>
+      <c r="BH15" s="1"/>
+      <c r="BI15" s="1"/>
+      <c r="BJ15" s="1"/>
+      <c r="BK15" s="1"/>
+      <c r="BL15" s="1"/>
+      <c r="BM15" s="1"/>
+      <c r="BN15" s="1"/>
+      <c r="BO15" s="1"/>
+      <c r="BP15" s="1"/>
+    </row>
+    <row r="16" spans="1:68" ht="13.5" customHeight="1">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="18" t="s">
+        <v>1</v>
       </c>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="1"/>
+      <c r="AD16" s="1"/>
+      <c r="AE16" s="1"/>
+      <c r="AF16" s="1"/>
+      <c r="AG16" s="1"/>
+      <c r="AH16" s="1"/>
+      <c r="AI16" s="1"/>
+      <c r="AJ16" s="1"/>
+      <c r="AK16" s="1"/>
+      <c r="AL16" s="1"/>
+      <c r="AM16" s="1"/>
+      <c r="AN16" s="1"/>
+      <c r="AO16" s="1"/>
+      <c r="AP16" s="1"/>
+      <c r="AQ16" s="1"/>
+      <c r="AR16" s="1"/>
+      <c r="AS16" s="1"/>
+      <c r="AT16" s="1"/>
+      <c r="AU16" s="1"/>
+      <c r="AV16" s="1"/>
+      <c r="AW16" s="1"/>
+      <c r="AX16" s="1"/>
+      <c r="AY16" s="1"/>
+      <c r="AZ16" s="1"/>
+      <c r="BA16" s="1"/>
+      <c r="BB16" s="1"/>
+      <c r="BC16" s="1"/>
+      <c r="BD16" s="1"/>
+      <c r="BE16" s="1"/>
+      <c r="BF16" s="1"/>
+      <c r="BG16" s="1"/>
+      <c r="BH16" s="1"/>
+      <c r="BI16" s="1"/>
+      <c r="BJ16" s="1"/>
+      <c r="BK16" s="1"/>
+      <c r="BL16" s="1"/>
+      <c r="BM16" s="1"/>
+      <c r="BN16" s="1"/>
+      <c r="BO16" s="1"/>
+      <c r="BP16" s="1"/>
+    </row>
+    <row r="17" spans="1:68" ht="13.5" customHeight="1">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="1"/>
+      <c r="AD17" s="1"/>
+      <c r="AE17" s="1"/>
+      <c r="AF17" s="1"/>
+      <c r="AG17" s="1"/>
+      <c r="AH17" s="1"/>
+      <c r="AI17" s="1"/>
+      <c r="AJ17" s="1"/>
+      <c r="AK17" s="1"/>
+      <c r="AL17" s="1"/>
+      <c r="AM17" s="1"/>
+      <c r="AN17" s="1"/>
+      <c r="AO17" s="1"/>
+      <c r="AP17" s="1"/>
+      <c r="AQ17" s="1"/>
+      <c r="AR17" s="1"/>
+      <c r="AS17" s="1"/>
+      <c r="AT17" s="1"/>
+      <c r="AU17" s="1"/>
+      <c r="AV17" s="1"/>
+      <c r="AW17" s="1"/>
+      <c r="AX17" s="1"/>
+      <c r="AY17" s="1"/>
+      <c r="AZ17" s="1"/>
+      <c r="BA17" s="1"/>
+      <c r="BB17" s="1"/>
+      <c r="BC17" s="1"/>
+      <c r="BD17" s="1"/>
+      <c r="BE17" s="1"/>
+      <c r="BF17" s="1"/>
+      <c r="BG17" s="1"/>
+      <c r="BH17" s="1"/>
+      <c r="BI17" s="1"/>
+      <c r="BJ17" s="1"/>
+      <c r="BK17" s="1"/>
+      <c r="BL17" s="1"/>
+      <c r="BM17" s="1"/>
+      <c r="BN17" s="1"/>
+      <c r="BO17" s="1"/>
+      <c r="BP17" s="1"/>
+    </row>
+    <row r="18" spans="1:68">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="1"/>
+      <c r="AD18" s="1"/>
+      <c r="AE18" s="1"/>
+      <c r="AF18" s="1"/>
+      <c r="AG18" s="1"/>
+      <c r="AH18" s="1"/>
+      <c r="AI18" s="1"/>
+      <c r="AJ18" s="1"/>
+      <c r="AK18" s="1"/>
+      <c r="AL18" s="1"/>
+      <c r="AM18" s="1"/>
+      <c r="AN18" s="1"/>
+      <c r="AO18" s="1"/>
+      <c r="AP18" s="1"/>
+      <c r="AQ18" s="1"/>
+      <c r="AR18" s="1"/>
+      <c r="AS18" s="1"/>
+      <c r="AT18" s="1"/>
+      <c r="AU18" s="1"/>
+      <c r="AV18" s="1"/>
+      <c r="AW18" s="1"/>
+      <c r="AX18" s="1"/>
+      <c r="AY18" s="1"/>
+      <c r="AZ18" s="1"/>
+      <c r="BA18" s="1"/>
+      <c r="BB18" s="1"/>
+      <c r="BC18" s="1"/>
+      <c r="BD18" s="1"/>
+      <c r="BE18" s="1"/>
+      <c r="BF18" s="1"/>
+      <c r="BG18" s="1"/>
+      <c r="BH18" s="1"/>
+      <c r="BI18" s="1"/>
+      <c r="BJ18" s="1"/>
+      <c r="BK18" s="1"/>
+      <c r="BL18" s="1"/>
+      <c r="BM18" s="1"/>
+      <c r="BN18" s="1"/>
+      <c r="BO18" s="1"/>
+      <c r="BP18" s="1"/>
+    </row>
+    <row r="19" spans="1:68" ht="13.5" customHeight="1">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1"/>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="1"/>
+      <c r="AC19" s="1"/>
+      <c r="AD19" s="1"/>
+      <c r="AE19" s="1"/>
+      <c r="AF19" s="1"/>
+      <c r="AG19" s="1"/>
+      <c r="AH19" s="1"/>
+      <c r="AI19" s="1"/>
+      <c r="AJ19" s="1"/>
+      <c r="AK19" s="1"/>
+      <c r="AL19" s="1"/>
+      <c r="AM19" s="1"/>
+      <c r="AN19" s="1"/>
+      <c r="AO19" s="1"/>
+      <c r="AP19" s="1"/>
+      <c r="AQ19" s="1"/>
+      <c r="AR19" s="1"/>
+      <c r="AS19" s="1"/>
+      <c r="AT19" s="1"/>
+      <c r="AU19" s="1"/>
+      <c r="AV19" s="1"/>
+      <c r="AW19" s="1"/>
+      <c r="AX19" s="1"/>
+      <c r="AY19" s="1"/>
+      <c r="AZ19" s="1"/>
+      <c r="BA19" s="1"/>
+      <c r="BB19" s="1"/>
+      <c r="BC19" s="1"/>
+      <c r="BD19" s="1"/>
+      <c r="BE19" s="1"/>
+      <c r="BF19" s="1"/>
+      <c r="BG19" s="1"/>
+      <c r="BH19" s="1"/>
+      <c r="BI19" s="1"/>
+      <c r="BJ19" s="1"/>
+      <c r="BK19" s="1"/>
+      <c r="BL19" s="1"/>
+      <c r="BM19" s="1"/>
+      <c r="BN19" s="1"/>
+      <c r="BO19" s="1"/>
+      <c r="BP19" s="1"/>
+    </row>
+    <row r="20" spans="1:68" ht="13.5" customHeight="1">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="1"/>
+      <c r="AD20" s="1"/>
+      <c r="AE20" s="1"/>
+      <c r="AF20" s="1"/>
+      <c r="AG20" s="1"/>
+      <c r="AH20" s="1"/>
+      <c r="AI20" s="1"/>
+      <c r="AJ20" s="1"/>
+      <c r="AK20" s="1"/>
+      <c r="AL20" s="1"/>
+      <c r="AM20" s="1"/>
+      <c r="AN20" s="1"/>
+      <c r="AO20" s="1"/>
+      <c r="AP20" s="1"/>
+      <c r="AQ20" s="1"/>
+      <c r="AR20" s="1"/>
+      <c r="AS20" s="1"/>
+      <c r="AT20" s="1"/>
+      <c r="AU20" s="1"/>
+      <c r="AV20" s="1"/>
+      <c r="AW20" s="1"/>
+      <c r="AX20" s="1"/>
+      <c r="AY20" s="1"/>
+      <c r="AZ20" s="1"/>
+      <c r="BA20" s="1"/>
+      <c r="BB20" s="1"/>
+      <c r="BC20" s="1"/>
+      <c r="BD20" s="1"/>
+      <c r="BE20" s="1"/>
+      <c r="BF20" s="1"/>
+      <c r="BG20" s="1"/>
+      <c r="BH20" s="1"/>
+      <c r="BI20" s="1"/>
+      <c r="BJ20" s="1"/>
+      <c r="BK20" s="1"/>
+      <c r="BL20" s="1"/>
+      <c r="BM20" s="1"/>
+      <c r="BN20" s="1"/>
+      <c r="BO20" s="1"/>
+      <c r="BP20" s="1"/>
+    </row>
+    <row r="21" spans="1:68">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="1"/>
+      <c r="AC21" s="1"/>
+      <c r="AD21" s="1"/>
+      <c r="AE21" s="1"/>
+      <c r="AF21" s="1"/>
+      <c r="AG21" s="1"/>
+      <c r="AH21" s="1"/>
+      <c r="AI21" s="1"/>
+      <c r="AJ21" s="1"/>
+      <c r="AK21" s="1"/>
+      <c r="AL21" s="1"/>
+      <c r="AM21" s="1"/>
+      <c r="AN21" s="1"/>
+      <c r="AO21" s="1"/>
+      <c r="AP21" s="1"/>
+      <c r="AQ21" s="1"/>
+      <c r="AR21" s="1"/>
+      <c r="AS21" s="1"/>
+      <c r="AT21" s="1"/>
+      <c r="AU21" s="1"/>
+      <c r="AV21" s="1"/>
+      <c r="AW21" s="1"/>
+      <c r="AX21" s="1"/>
+      <c r="AY21" s="1"/>
+      <c r="AZ21" s="1"/>
+      <c r="BA21" s="1"/>
+      <c r="BB21" s="1"/>
+      <c r="BC21" s="1"/>
+      <c r="BD21" s="1"/>
+      <c r="BE21" s="1"/>
+      <c r="BF21" s="1"/>
+      <c r="BG21" s="1"/>
+      <c r="BH21" s="1"/>
+      <c r="BI21" s="1"/>
+      <c r="BJ21" s="1"/>
+      <c r="BK21" s="1"/>
+      <c r="BL21" s="1"/>
+      <c r="BM21" s="1"/>
+      <c r="BN21" s="1"/>
+      <c r="BO21" s="1"/>
+      <c r="BP21" s="1"/>
+    </row>
+    <row r="22" spans="1:68">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1"/>
+      <c r="AA22" s="1"/>
+      <c r="AB22" s="1"/>
+      <c r="AC22" s="1"/>
+      <c r="AD22" s="1"/>
+      <c r="AE22" s="1"/>
+      <c r="AF22" s="1"/>
+      <c r="AG22" s="1"/>
+      <c r="AH22" s="1"/>
+      <c r="AI22" s="1"/>
+      <c r="AJ22" s="1"/>
+      <c r="AK22" s="1"/>
+      <c r="AL22" s="1"/>
+      <c r="AM22" s="1"/>
+      <c r="AN22" s="1"/>
+      <c r="AO22" s="1"/>
+      <c r="AP22" s="1"/>
+      <c r="AQ22" s="1"/>
+      <c r="AR22" s="1"/>
+      <c r="AS22" s="1"/>
+      <c r="AT22" s="1"/>
+      <c r="AU22" s="1"/>
+      <c r="AV22" s="1"/>
+      <c r="AW22" s="1"/>
+      <c r="AX22" s="1"/>
+      <c r="AY22" s="1"/>
+      <c r="AZ22" s="1"/>
+      <c r="BA22" s="1"/>
+      <c r="BB22" s="1"/>
+      <c r="BC22" s="1"/>
+      <c r="BD22" s="1"/>
+      <c r="BE22" s="1"/>
+      <c r="BF22" s="1"/>
+      <c r="BG22" s="1"/>
+      <c r="BH22" s="1"/>
+      <c r="BI22" s="1"/>
+      <c r="BJ22" s="1"/>
+      <c r="BK22" s="1"/>
+      <c r="BL22" s="1"/>
+      <c r="BM22" s="1"/>
+      <c r="BN22" s="1"/>
+      <c r="BO22" s="1"/>
+      <c r="BP22" s="1"/>
+    </row>
+    <row r="26" spans="1:68">
+      <c r="L26" t="s">
+        <v>91</v>
+      </c>
+      <c r="M26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:68">
+      <c r="M27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:68">
+      <c r="M28" s="17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:68">
+      <c r="L30" t="s">
+        <v>91</v>
+      </c>
+      <c r="M30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:68">
+      <c r="L32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="12:12">
+      <c r="L33" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C16:H17"/>
+    <mergeCell ref="C19:H20"/>
+    <mergeCell ref="C6:H7"/>
+    <mergeCell ref="C9:H10"/>
+  </mergeCells>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:BP28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.25" defaultRowHeight="13.5"/>
+  <sheetData>
+    <row r="1" spans="1:68">
+      <c r="A1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:68">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1"/>
+      <c r="AL2" s="1"/>
+      <c r="AM2" s="1"/>
+      <c r="AN2" s="1"/>
+      <c r="AO2" s="1"/>
+      <c r="AP2" s="1"/>
+      <c r="AQ2" s="1"/>
+      <c r="AR2" s="1"/>
+      <c r="AS2" s="1"/>
+      <c r="AT2" s="1"/>
+      <c r="AU2" s="1"/>
+      <c r="AV2" s="1"/>
+      <c r="AW2" s="1"/>
+      <c r="AX2" s="1"/>
+      <c r="AY2" s="1"/>
+      <c r="AZ2" s="1"/>
+      <c r="BA2" s="1"/>
+      <c r="BB2" s="1"/>
+      <c r="BC2" s="1"/>
+      <c r="BD2" s="1"/>
+      <c r="BE2" s="1"/>
+      <c r="BF2" s="1"/>
+      <c r="BG2" s="1"/>
+      <c r="BH2" s="1"/>
+      <c r="BI2" s="1"/>
+      <c r="BJ2" s="1"/>
+      <c r="BK2" s="1"/>
+      <c r="BL2" s="1"/>
+      <c r="BM2" s="1"/>
+      <c r="BN2" s="1"/>
+      <c r="BO2" s="1"/>
+      <c r="BP2" s="1"/>
+    </row>
+    <row r="3" spans="1:68">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AI3" s="1"/>
+      <c r="AJ3" s="1"/>
+      <c r="AK3" s="1"/>
+      <c r="AL3" s="1"/>
+      <c r="AM3" s="1"/>
+      <c r="AN3" s="1"/>
+      <c r="AO3" s="1"/>
+      <c r="AP3" s="1"/>
+      <c r="AQ3" s="1"/>
+      <c r="AR3" s="1"/>
+      <c r="AS3" s="1"/>
+      <c r="AT3" s="1"/>
+      <c r="AU3" s="1"/>
+      <c r="AV3" s="1"/>
+      <c r="AW3" s="1"/>
+      <c r="AX3" s="1"/>
+      <c r="AY3" s="1"/>
+      <c r="AZ3" s="1"/>
+      <c r="BA3" s="1"/>
+      <c r="BB3" s="1"/>
+      <c r="BC3" s="1"/>
+      <c r="BD3" s="1"/>
+      <c r="BE3" s="1"/>
+      <c r="BF3" s="1"/>
+      <c r="BG3" s="1"/>
+      <c r="BH3" s="1"/>
+      <c r="BI3" s="1"/>
+      <c r="BJ3" s="1"/>
+      <c r="BK3" s="1"/>
+      <c r="BL3" s="1"/>
+      <c r="BM3" s="1"/>
+      <c r="BN3" s="1"/>
+      <c r="BO3" s="1"/>
+      <c r="BP3" s="1"/>
+    </row>
+    <row r="4" spans="1:68">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1"/>
+      <c r="AG4" s="1"/>
+      <c r="AH4" s="1"/>
+      <c r="AI4" s="1"/>
+      <c r="AJ4" s="1"/>
+      <c r="AK4" s="1"/>
+      <c r="AL4" s="1"/>
+      <c r="AM4" s="1"/>
+      <c r="AN4" s="1"/>
+      <c r="AO4" s="1"/>
+      <c r="AP4" s="1"/>
+      <c r="AQ4" s="1"/>
+      <c r="AR4" s="1"/>
+      <c r="AS4" s="1"/>
+      <c r="AT4" s="1"/>
+      <c r="AU4" s="1"/>
+      <c r="AV4" s="1"/>
+      <c r="AW4" s="1"/>
+      <c r="AX4" s="1"/>
+      <c r="AY4" s="1"/>
+      <c r="AZ4" s="1"/>
+      <c r="BA4" s="1"/>
+      <c r="BB4" s="1"/>
+      <c r="BC4" s="1"/>
+      <c r="BD4" s="1"/>
+      <c r="BE4" s="1"/>
+      <c r="BF4" s="1"/>
+      <c r="BG4" s="1"/>
+      <c r="BH4" s="1"/>
+      <c r="BI4" s="1"/>
+      <c r="BJ4" s="1"/>
+      <c r="BK4" s="1"/>
+      <c r="BL4" s="1"/>
+      <c r="BM4" s="1"/>
+      <c r="BN4" s="1"/>
+      <c r="BO4" s="1"/>
+      <c r="BP4" s="1"/>
+    </row>
+    <row r="5" spans="1:68">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1"/>
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1"/>
+      <c r="AI5" s="1"/>
+      <c r="AJ5" s="1"/>
+      <c r="AK5" s="1"/>
+      <c r="AL5" s="1"/>
+      <c r="AM5" s="1"/>
+      <c r="AN5" s="1"/>
+      <c r="AO5" s="1"/>
+      <c r="AP5" s="1"/>
+      <c r="AQ5" s="1"/>
+      <c r="AR5" s="1"/>
+      <c r="AS5" s="1"/>
+      <c r="AT5" s="1"/>
+      <c r="AU5" s="1"/>
+      <c r="AV5" s="1"/>
+      <c r="AW5" s="1"/>
+      <c r="AX5" s="1"/>
+      <c r="AY5" s="1"/>
+      <c r="AZ5" s="1"/>
+      <c r="BA5" s="1"/>
+      <c r="BB5" s="1"/>
+      <c r="BC5" s="1"/>
+      <c r="BD5" s="1"/>
+      <c r="BE5" s="1"/>
+      <c r="BF5" s="1"/>
+      <c r="BG5" s="1"/>
+      <c r="BH5" s="1"/>
+      <c r="BI5" s="1"/>
+      <c r="BJ5" s="1"/>
+      <c r="BK5" s="1"/>
+      <c r="BL5" s="1"/>
+      <c r="BM5" s="1"/>
+      <c r="BN5" s="1"/>
+      <c r="BO5" s="1"/>
+      <c r="BP5" s="1"/>
+    </row>
+    <row r="6" spans="1:68">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="1"/>
+      <c r="AG6" s="1"/>
+      <c r="AH6" s="1"/>
+      <c r="AI6" s="1"/>
+      <c r="AJ6" s="1"/>
+      <c r="AK6" s="1"/>
+      <c r="AL6" s="1"/>
+      <c r="AM6" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN6" s="19"/>
+      <c r="AO6" s="19"/>
+      <c r="AP6" s="19"/>
+      <c r="AQ6" s="1"/>
+      <c r="AR6" s="1"/>
+      <c r="AS6" s="1"/>
+      <c r="AT6" s="1"/>
+      <c r="AU6" s="1"/>
+      <c r="AV6" s="1"/>
+      <c r="AW6" s="1"/>
+      <c r="AX6" s="1"/>
+      <c r="AY6" s="1"/>
+      <c r="AZ6" s="1"/>
+      <c r="BA6" s="1"/>
+      <c r="BB6" s="1"/>
+      <c r="BC6" s="1"/>
+      <c r="BD6" s="1"/>
+      <c r="BE6" s="1"/>
+      <c r="BF6" s="1"/>
+      <c r="BG6" s="1"/>
+      <c r="BH6" s="1"/>
+      <c r="BI6" s="1"/>
+      <c r="BJ6" s="1"/>
+      <c r="BK6" s="1"/>
+      <c r="BL6" s="1"/>
+      <c r="BM6" s="1"/>
+      <c r="BN6" s="1"/>
+      <c r="BO6" s="1"/>
+      <c r="BP6" s="1"/>
+    </row>
+    <row r="7" spans="1:68">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="1"/>
+      <c r="AG7" s="1"/>
+      <c r="AH7" s="1"/>
+      <c r="AI7" s="1"/>
+      <c r="AJ7" s="1"/>
+      <c r="AK7" s="1"/>
+      <c r="AL7" s="1"/>
+      <c r="AM7" s="19"/>
+      <c r="AN7" s="19"/>
+      <c r="AO7" s="19"/>
+      <c r="AP7" s="19"/>
+      <c r="AQ7" s="1"/>
+      <c r="AR7" s="1"/>
+      <c r="AS7" s="1"/>
+      <c r="AT7" s="1"/>
+      <c r="AU7" s="1"/>
+      <c r="AV7" s="1"/>
+      <c r="AW7" s="1"/>
+      <c r="AX7" s="1"/>
+      <c r="AY7" s="1"/>
+      <c r="AZ7" s="1"/>
+      <c r="BA7" s="1"/>
+      <c r="BB7" s="1"/>
+      <c r="BC7" s="1"/>
+      <c r="BD7" s="1"/>
+      <c r="BE7" s="1"/>
+      <c r="BF7" s="1"/>
+      <c r="BG7" s="1"/>
+      <c r="BH7" s="1"/>
+      <c r="BI7" s="1"/>
+      <c r="BJ7" s="1"/>
+      <c r="BK7" s="1"/>
+      <c r="BL7" s="1"/>
+      <c r="BM7" s="1"/>
+      <c r="BN7" s="1"/>
+      <c r="BO7" s="1"/>
+      <c r="BP7" s="1"/>
+    </row>
+    <row r="8" spans="1:68">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="1"/>
+      <c r="AG8" s="1"/>
+      <c r="AH8" s="1"/>
+      <c r="AI8" s="1"/>
+      <c r="AJ8" s="1"/>
+      <c r="AK8" s="1"/>
+      <c r="AL8" s="1"/>
+      <c r="AM8" s="1"/>
+      <c r="AN8" s="1"/>
+      <c r="AO8" s="1"/>
+      <c r="AP8" s="1"/>
+      <c r="AQ8" s="1"/>
+      <c r="AR8" s="1"/>
+      <c r="AS8" s="1"/>
+      <c r="AT8" s="1"/>
+      <c r="AU8" s="1"/>
+      <c r="AV8" s="1"/>
+      <c r="AW8" s="1"/>
+      <c r="AX8" s="1"/>
+      <c r="AY8" s="1"/>
+      <c r="AZ8" s="1"/>
+      <c r="BA8" s="1"/>
+      <c r="BB8" s="1"/>
+      <c r="BC8" s="1"/>
+      <c r="BD8" s="1"/>
+      <c r="BE8" s="1"/>
+      <c r="BF8" s="1"/>
+      <c r="BG8" s="1"/>
+      <c r="BH8" s="1"/>
+      <c r="BI8" s="1"/>
+      <c r="BJ8" s="1"/>
+      <c r="BK8" s="1"/>
+      <c r="BL8" s="1"/>
+      <c r="BM8" s="1"/>
+      <c r="BN8" s="1"/>
+      <c r="BO8" s="1"/>
+      <c r="BP8" s="1"/>
+    </row>
+    <row r="9" spans="1:68" ht="13.5" customHeight="1">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
+      <c r="AE9" s="1"/>
+      <c r="AF9" s="1"/>
+      <c r="AG9" s="1"/>
+      <c r="AH9" s="1"/>
+      <c r="AI9" s="1"/>
+      <c r="AJ9" s="1"/>
+      <c r="AK9" s="1"/>
+      <c r="AL9" s="1"/>
+      <c r="AM9" s="1"/>
+      <c r="AN9" s="1"/>
+      <c r="AO9" s="1"/>
+      <c r="AP9" s="1"/>
+      <c r="AQ9" s="1"/>
+      <c r="AR9" s="1"/>
+      <c r="AS9" s="1"/>
+      <c r="AT9" s="1"/>
+      <c r="AU9" s="1"/>
+      <c r="AV9" s="1"/>
+      <c r="AW9" s="1"/>
+      <c r="AX9" s="1"/>
+      <c r="AY9" s="1"/>
+      <c r="AZ9" s="1"/>
+      <c r="BA9" s="1"/>
+      <c r="BB9" s="1"/>
+      <c r="BC9" s="1"/>
+      <c r="BD9" s="1"/>
+      <c r="BE9" s="1"/>
+      <c r="BF9" s="1"/>
+      <c r="BG9" s="1"/>
+      <c r="BH9" s="1"/>
+      <c r="BI9" s="1"/>
+      <c r="BJ9" s="1"/>
+      <c r="BK9" s="1"/>
+      <c r="BL9" s="1"/>
+      <c r="BM9" s="1"/>
+      <c r="BN9" s="1"/>
+      <c r="BO9" s="1"/>
+      <c r="BP9" s="1"/>
+    </row>
+    <row r="10" spans="1:68" ht="13.5" customHeight="1">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="1"/>
+      <c r="AE10" s="1"/>
+      <c r="AF10" s="1"/>
+      <c r="AG10" s="1"/>
+      <c r="AH10" s="1"/>
+      <c r="AI10" s="1"/>
+      <c r="AJ10" s="1"/>
+      <c r="AK10" s="1"/>
+      <c r="AL10" s="1"/>
+      <c r="AM10" s="1"/>
+      <c r="AN10" s="1"/>
+      <c r="AO10" s="1"/>
+      <c r="AP10" s="1"/>
+      <c r="AQ10" s="1"/>
+      <c r="AR10" s="1"/>
+      <c r="AS10" s="1"/>
+      <c r="AT10" s="1"/>
+      <c r="AU10" s="1"/>
+      <c r="AV10" s="1"/>
+      <c r="AW10" s="1"/>
+      <c r="AX10" s="1"/>
+      <c r="AY10" s="1"/>
+      <c r="AZ10" s="1"/>
+      <c r="BA10" s="1"/>
+      <c r="BB10" s="1"/>
+      <c r="BC10" s="1"/>
+      <c r="BD10" s="1"/>
+      <c r="BE10" s="1"/>
+      <c r="BF10" s="1"/>
+      <c r="BG10" s="1"/>
+      <c r="BH10" s="1"/>
+      <c r="BI10" s="1"/>
+      <c r="BJ10" s="1"/>
+      <c r="BK10" s="1"/>
+      <c r="BL10" s="1"/>
+      <c r="BM10" s="1"/>
+      <c r="BN10" s="1"/>
+      <c r="BO10" s="1"/>
+      <c r="BP10" s="1"/>
+    </row>
+    <row r="11" spans="1:68">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="1"/>
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="1"/>
+      <c r="AG11" s="1"/>
+      <c r="AH11" s="1"/>
+      <c r="AI11" s="1"/>
+      <c r="AJ11" s="1"/>
+      <c r="AK11" s="1"/>
+      <c r="AL11" s="1"/>
+      <c r="AM11" s="1"/>
+      <c r="AN11" s="1"/>
+      <c r="AO11" s="1"/>
+      <c r="AP11" s="1"/>
+      <c r="AQ11" s="1"/>
+      <c r="AR11" s="1"/>
+      <c r="AS11" s="1"/>
+      <c r="AT11" s="1"/>
+      <c r="AU11" s="1"/>
+      <c r="AV11" s="1"/>
+      <c r="AW11" s="1"/>
+      <c r="AX11" s="1"/>
+      <c r="AY11" s="1"/>
+      <c r="AZ11" s="1"/>
+      <c r="BA11" s="1"/>
+      <c r="BB11" s="1"/>
+      <c r="BC11" s="1"/>
+      <c r="BD11" s="1"/>
+      <c r="BE11" s="1"/>
+      <c r="BF11" s="1"/>
+      <c r="BG11" s="1"/>
+      <c r="BH11" s="1"/>
+      <c r="BI11" s="1"/>
+      <c r="BJ11" s="1"/>
+      <c r="BK11" s="1"/>
+      <c r="BL11" s="1"/>
+      <c r="BM11" s="1"/>
+      <c r="BN11" s="1"/>
+      <c r="BO11" s="1"/>
+      <c r="BP11" s="1"/>
+    </row>
+    <row r="12" spans="1:68" ht="13.5" customHeight="1">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
+      <c r="AD12" s="1"/>
+      <c r="AE12" s="1"/>
+      <c r="AF12" s="1"/>
+      <c r="AG12" s="1"/>
+      <c r="AH12" s="1"/>
+      <c r="AI12" s="1"/>
+      <c r="AJ12" s="1"/>
+      <c r="AK12" s="1"/>
+      <c r="AL12" s="1"/>
+      <c r="AM12" s="1"/>
+      <c r="AN12" s="1"/>
+      <c r="AO12" s="1"/>
+      <c r="AP12" s="1"/>
+      <c r="AQ12" s="1"/>
+      <c r="AR12" s="1"/>
+      <c r="AS12" s="1"/>
+      <c r="AT12" s="1"/>
+      <c r="AU12" s="1"/>
+      <c r="AV12" s="1"/>
+      <c r="AW12" s="1"/>
+      <c r="AX12" s="1"/>
+      <c r="AY12" s="1"/>
+      <c r="AZ12" s="1"/>
+      <c r="BA12" s="1"/>
+      <c r="BB12" s="1"/>
+      <c r="BC12" s="1"/>
+      <c r="BD12" s="1"/>
+      <c r="BE12" s="1"/>
+      <c r="BF12" s="1"/>
+      <c r="BG12" s="1"/>
+      <c r="BH12" s="1"/>
+      <c r="BI12" s="1"/>
+      <c r="BJ12" s="1"/>
+      <c r="BK12" s="1"/>
+      <c r="BL12" s="1"/>
+      <c r="BM12" s="1"/>
+      <c r="BN12" s="1"/>
+      <c r="BO12" s="1"/>
+      <c r="BP12" s="1"/>
+    </row>
+    <row r="13" spans="1:68" ht="13.5" customHeight="1">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="1"/>
+      <c r="AD13" s="1"/>
+      <c r="AE13" s="1"/>
+      <c r="AF13" s="1"/>
+      <c r="AG13" s="1"/>
+      <c r="AH13" s="1"/>
+      <c r="AI13" s="1"/>
+      <c r="AJ13" s="1"/>
+      <c r="AK13" s="1"/>
+      <c r="AL13" s="1"/>
+      <c r="AM13" s="1"/>
+      <c r="AN13" s="1"/>
+      <c r="AO13" s="1"/>
+      <c r="AP13" s="1"/>
+      <c r="AQ13" s="1"/>
+      <c r="AR13" s="1"/>
+      <c r="AS13" s="1"/>
+      <c r="AT13" s="1"/>
+      <c r="AU13" s="1"/>
+      <c r="AV13" s="1"/>
+      <c r="AW13" s="1"/>
+      <c r="AX13" s="1"/>
+      <c r="AY13" s="1"/>
+      <c r="AZ13" s="1"/>
+      <c r="BA13" s="1"/>
+      <c r="BB13" s="1"/>
+      <c r="BC13" s="1"/>
+      <c r="BD13" s="1"/>
+      <c r="BE13" s="1"/>
+      <c r="BF13" s="1"/>
+      <c r="BG13" s="1"/>
+      <c r="BH13" s="1"/>
+      <c r="BI13" s="1"/>
+      <c r="BJ13" s="1"/>
+      <c r="BK13" s="1"/>
+      <c r="BL13" s="1"/>
+      <c r="BM13" s="1"/>
+      <c r="BN13" s="1"/>
+      <c r="BO13" s="1"/>
+      <c r="BP13" s="1"/>
+    </row>
+    <row r="14" spans="1:68">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="1"/>
+      <c r="AE14" s="1"/>
+      <c r="AF14" s="1"/>
+      <c r="AG14" s="1"/>
+      <c r="AH14" s="1"/>
+      <c r="AI14" s="1"/>
+      <c r="AJ14" s="1"/>
+      <c r="AK14" s="1"/>
+      <c r="AL14" s="1"/>
+      <c r="AM14" s="1"/>
+      <c r="AN14" s="1"/>
+      <c r="AO14" s="1"/>
+      <c r="AP14" s="1"/>
+      <c r="AQ14" s="1"/>
+      <c r="AR14" s="1"/>
+      <c r="AS14" s="1"/>
+      <c r="AT14" s="1"/>
+      <c r="AU14" s="1"/>
+      <c r="AV14" s="1"/>
+      <c r="AW14" s="1"/>
+      <c r="AX14" s="1"/>
+      <c r="AY14" s="1"/>
+      <c r="AZ14" s="1"/>
+      <c r="BA14" s="1"/>
+      <c r="BB14" s="1"/>
+      <c r="BC14" s="1"/>
+      <c r="BD14" s="1"/>
+      <c r="BE14" s="1"/>
+      <c r="BF14" s="1"/>
+      <c r="BG14" s="1"/>
+      <c r="BH14" s="1"/>
+      <c r="BI14" s="1"/>
+      <c r="BJ14" s="1"/>
+      <c r="BK14" s="1"/>
+      <c r="BL14" s="1"/>
+      <c r="BM14" s="1"/>
+      <c r="BN14" s="1"/>
+      <c r="BO14" s="1"/>
+      <c r="BP14" s="1"/>
+    </row>
+    <row r="15" spans="1:68">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -16587,7 +19488,9 @@
     </row>
     <row r="16" spans="1:68">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+      <c r="B16" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -16728,24 +19631,20 @@
     <row r="18" spans="1:68">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
@@ -16773,12 +19672,10 @@
       <c r="AO18" s="1"/>
       <c r="AP18" s="1"/>
       <c r="AQ18" s="1"/>
-      <c r="AR18" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="AS18" s="17"/>
-      <c r="AT18" s="17"/>
-      <c r="AU18" s="17"/>
+      <c r="AR18" s="1"/>
+      <c r="AS18" s="1"/>
+      <c r="AT18" s="1"/>
+      <c r="AU18" s="1"/>
       <c r="AV18" s="1"/>
       <c r="AW18" s="1"/>
       <c r="AX18" s="1"/>
@@ -16804,20 +19701,24 @@
     <row r="19" spans="1:68">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
+      <c r="C19" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="17"/>
-      <c r="P19" s="17"/>
+      <c r="M19" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="N19" s="19"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="19"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
@@ -16845,10 +19746,12 @@
       <c r="AO19" s="1"/>
       <c r="AP19" s="1"/>
       <c r="AQ19" s="1"/>
-      <c r="AR19" s="17"/>
-      <c r="AS19" s="17"/>
-      <c r="AT19" s="17"/>
-      <c r="AU19" s="17"/>
+      <c r="AR19" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS19" s="19"/>
+      <c r="AT19" s="19"/>
+      <c r="AU19" s="19"/>
       <c r="AV19" s="1"/>
       <c r="AW19" s="1"/>
       <c r="AX19" s="1"/>
@@ -16874,20 +19777,20 @@
     <row r="20" spans="1:68">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
@@ -16915,10 +19818,10 @@
       <c r="AO20" s="1"/>
       <c r="AP20" s="1"/>
       <c r="AQ20" s="1"/>
-      <c r="AR20" s="1"/>
-      <c r="AS20" s="1"/>
-      <c r="AT20" s="1"/>
-      <c r="AU20" s="1"/>
+      <c r="AR20" s="19"/>
+      <c r="AS20" s="19"/>
+      <c r="AT20" s="19"/>
+      <c r="AU20" s="19"/>
       <c r="AV20" s="1"/>
       <c r="AW20" s="1"/>
       <c r="AX20" s="1"/>
@@ -16941,17 +19844,15 @@
       <c r="BO20" s="1"/>
       <c r="BP20" s="1"/>
     </row>
-    <row r="21" spans="1:68" ht="13.5" customHeight="1">
+    <row r="21" spans="1:68">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -17016,7 +19917,9 @@
     <row r="22" spans="1:68" ht="13.5" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="18"/>
+      <c r="C22" s="18" t="s">
+        <v>1</v>
+      </c>
       <c r="D22" s="18"/>
       <c r="E22" s="18"/>
       <c r="F22" s="18"/>
@@ -17083,15 +19986,15 @@
       <c r="BO22" s="1"/>
       <c r="BP22" s="1"/>
     </row>
-    <row r="23" spans="1:68">
+    <row r="23" spans="1:68" ht="13.5" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -17153,17 +20056,15 @@
       <c r="BO23" s="1"/>
       <c r="BP23" s="1"/>
     </row>
-    <row r="24" spans="1:68" ht="13.5" customHeight="1">
+    <row r="24" spans="1:68">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -17228,7 +20129,9 @@
     <row r="25" spans="1:68" ht="13.5" customHeight="1">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="18"/>
+      <c r="C25" s="18" t="s">
+        <v>2</v>
+      </c>
       <c r="D25" s="18"/>
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
@@ -17295,15 +20198,15 @@
       <c r="BO25" s="1"/>
       <c r="BP25" s="1"/>
     </row>
-    <row r="26" spans="1:68">
+    <row r="26" spans="1:68" ht="13.5" customHeight="1">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -17435,18 +20338,88 @@
       <c r="BO27" s="1"/>
       <c r="BP27" s="1"/>
     </row>
+    <row r="28" spans="1:68">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
+      <c r="AA28" s="1"/>
+      <c r="AB28" s="1"/>
+      <c r="AC28" s="1"/>
+      <c r="AD28" s="1"/>
+      <c r="AE28" s="1"/>
+      <c r="AF28" s="1"/>
+      <c r="AG28" s="1"/>
+      <c r="AH28" s="1"/>
+      <c r="AI28" s="1"/>
+      <c r="AJ28" s="1"/>
+      <c r="AK28" s="1"/>
+      <c r="AL28" s="1"/>
+      <c r="AM28" s="1"/>
+      <c r="AN28" s="1"/>
+      <c r="AO28" s="1"/>
+      <c r="AP28" s="1"/>
+      <c r="AQ28" s="1"/>
+      <c r="AR28" s="1"/>
+      <c r="AS28" s="1"/>
+      <c r="AT28" s="1"/>
+      <c r="AU28" s="1"/>
+      <c r="AV28" s="1"/>
+      <c r="AW28" s="1"/>
+      <c r="AX28" s="1"/>
+      <c r="AY28" s="1"/>
+      <c r="AZ28" s="1"/>
+      <c r="BA28" s="1"/>
+      <c r="BB28" s="1"/>
+      <c r="BC28" s="1"/>
+      <c r="BD28" s="1"/>
+      <c r="BE28" s="1"/>
+      <c r="BF28" s="1"/>
+      <c r="BG28" s="1"/>
+      <c r="BH28" s="1"/>
+      <c r="BI28" s="1"/>
+      <c r="BJ28" s="1"/>
+      <c r="BK28" s="1"/>
+      <c r="BL28" s="1"/>
+      <c r="BM28" s="1"/>
+      <c r="BN28" s="1"/>
+      <c r="BO28" s="1"/>
+      <c r="BP28" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="AM5:AP6"/>
-    <mergeCell ref="AR18:AU19"/>
-    <mergeCell ref="C21:H22"/>
-    <mergeCell ref="C24:H25"/>
-    <mergeCell ref="C8:H9"/>
-    <mergeCell ref="C5:H6"/>
-    <mergeCell ref="C11:H12"/>
-    <mergeCell ref="M5:P6"/>
-    <mergeCell ref="C18:H19"/>
-    <mergeCell ref="M18:P19"/>
+    <mergeCell ref="AM6:AP7"/>
+    <mergeCell ref="AR19:AU20"/>
+    <mergeCell ref="C22:H23"/>
+    <mergeCell ref="C25:H26"/>
+    <mergeCell ref="C9:H10"/>
+    <mergeCell ref="C6:H7"/>
+    <mergeCell ref="C12:H13"/>
+    <mergeCell ref="M6:P7"/>
+    <mergeCell ref="C19:H20"/>
+    <mergeCell ref="M19:P20"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17455,12 +20428,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:O19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -17786,16 +20759,16 @@
       <c r="E14" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="F14" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="22"/>
       <c r="N14" s="5" t="s">
         <v>61</v>
       </c>
@@ -17810,16 +20783,16 @@
       <c r="E15" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
       <c r="N15" s="8"/>
       <c r="O15" s="1"/>
     </row>
@@ -17832,16 +20805,16 @@
       <c r="E16" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="F16" s="24" t="s">
+      <c r="F16" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="24"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
       <c r="N16" s="11" t="s">
         <v>83</v>
       </c>
@@ -17856,16 +20829,16 @@
       <c r="E17" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="23" t="s">
+      <c r="F17" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
       <c r="N17" s="14" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
update README(add Android App)
</commit_message>
<xml_diff>
--- a/doc/めも_IOエキスパンダー自作.xlsx
+++ b/doc/めも_IOエキスパンダー自作.xlsx
@@ -3437,6 +3437,1240 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="45" name="テキスト ボックス 44"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6724650" y="9269965"/>
+          <a:ext cx="1028700" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>Analog</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="正方形/長方形 34"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="485775" y="3124199"/>
+          <a:ext cx="2590800" cy="2190751"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>Host</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t> PC</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>or </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>Tablet via OTG</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>78340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="36" name="グループ化 35"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3067050" y="2992990"/>
+          <a:ext cx="1619250" cy="1283735"/>
+          <a:chOff x="3076575" y="535540"/>
+          <a:chExt cx="1619250" cy="1283735"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="37" name="直線コネクタ 36"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3076575" y="1819275"/>
+            <a:ext cx="1619250" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="28575">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="46" name="テキスト ボックス 45"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3238500" y="1554715"/>
+            <a:ext cx="1371600" cy="264560"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+              <a:t>USB</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="47" name="テキスト ボックス 46"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3200400" y="535540"/>
+            <a:ext cx="1371600" cy="264560"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+              <a:t>or</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="正方形/長方形 47"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="485775" y="6315074"/>
+          <a:ext cx="2590800" cy="2190751"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Host</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> PC</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1800" b="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>or </a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1800" b="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Tablet via OTG</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1400" b="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="49" name="正方形/長方形 48"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4695825" y="6172199"/>
+          <a:ext cx="1943100" cy="4476751"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>IO Expander MCU</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>60</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="正方形/長方形 49"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7915275" y="6286500"/>
+          <a:ext cx="1943100" cy="1019175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>e.g.LED,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>push-button </a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>109538</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>57152</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="直線コネクタ 50"/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="50" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6629400" y="6796088"/>
+          <a:ext cx="1285875" cy="633414"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1028700" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="52" name="テキスト ボックス 51"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6705600" y="6762750"/>
+          <a:ext cx="1028700" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>Digital</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t>  I/O</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>61</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="53" name="正方形/長方形 52"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7934325" y="9391650"/>
+          <a:ext cx="1943100" cy="809625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>e.g. Battery</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="54" name="直線コネクタ 53"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="61" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6638925" y="8201025"/>
+          <a:ext cx="1295400" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>21190</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1028700" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="55" name="テキスト ボックス 54"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6734175" y="8079340"/>
+          <a:ext cx="1028700" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>I2C</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>2911</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>148017</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="56" name="図 55" descr="ArduinoNano.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5184511" y="8377617"/>
+          <a:ext cx="921014" cy="2195133"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>121426</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>16651</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>60047</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="57" name="図 56" descr="ArduinoProMini.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5141101" y="6531751"/>
+          <a:ext cx="964424" cy="1757896"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>21190</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="58" name="グループ化 57"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3067050" y="12708490"/>
+          <a:ext cx="1619250" cy="264560"/>
+          <a:chOff x="3076575" y="1554715"/>
+          <a:chExt cx="1619250" cy="264560"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="59" name="直線コネクタ 58"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3076575" y="1819275"/>
+            <a:ext cx="1619250" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="28575">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="60" name="テキスト ボックス 59"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3238500" y="1554715"/>
+            <a:ext cx="1371600" cy="264560"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+              <a:t>USB</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>61</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="61" name="正方形/長方形 60"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7934325" y="7658100"/>
+          <a:ext cx="1943100" cy="1085850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>e.g. temperature</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>sensor</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="Meiryo UI" pitchFamily="50" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>23813</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="62" name="直線コネクタ 61"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="53" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="6657975" y="9391651"/>
+          <a:ext cx="1276350" cy="404812"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>11665</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1028700" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="63" name="テキスト ボックス 62"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -13613,10 +14847,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:BT64"/>
+  <dimension ref="A2:BT96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="S59" sqref="S59"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66:BT96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.125" defaultRowHeight="13.5"/>
@@ -18208,6 +19442,2300 @@
       <c r="BR64" s="1"/>
       <c r="BS64" s="1"/>
       <c r="BT64" s="1"/>
+    </row>
+    <row r="66" spans="1:72">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+      <c r="O66" s="1"/>
+      <c r="P66" s="1"/>
+      <c r="Q66" s="1"/>
+      <c r="R66" s="1"/>
+      <c r="S66" s="1"/>
+      <c r="T66" s="1"/>
+      <c r="U66" s="1"/>
+      <c r="V66" s="1"/>
+      <c r="W66" s="1"/>
+      <c r="X66" s="1"/>
+      <c r="Y66" s="1"/>
+      <c r="Z66" s="1"/>
+      <c r="AA66" s="1"/>
+      <c r="AB66" s="1"/>
+      <c r="AC66" s="1"/>
+      <c r="AD66" s="1"/>
+      <c r="AE66" s="1"/>
+      <c r="AF66" s="1"/>
+      <c r="AG66" s="1"/>
+      <c r="AH66" s="1"/>
+      <c r="AI66" s="1"/>
+      <c r="AJ66" s="1"/>
+      <c r="AK66" s="1"/>
+      <c r="AL66" s="1"/>
+      <c r="AM66" s="1"/>
+      <c r="AN66" s="1"/>
+      <c r="AO66" s="1"/>
+      <c r="AP66" s="1"/>
+      <c r="AQ66" s="1"/>
+      <c r="AR66" s="1"/>
+      <c r="AS66" s="1"/>
+      <c r="AT66" s="1"/>
+      <c r="AU66" s="1"/>
+      <c r="AV66" s="1"/>
+      <c r="AW66" s="1"/>
+      <c r="AX66" s="1"/>
+      <c r="AY66" s="1"/>
+      <c r="AZ66" s="1"/>
+      <c r="BA66" s="1"/>
+      <c r="BB66" s="1"/>
+      <c r="BC66" s="1"/>
+      <c r="BD66" s="1"/>
+      <c r="BE66" s="1"/>
+      <c r="BF66" s="1"/>
+      <c r="BG66" s="1"/>
+      <c r="BH66" s="1"/>
+      <c r="BI66" s="1"/>
+      <c r="BJ66" s="1"/>
+      <c r="BK66" s="1"/>
+      <c r="BL66" s="1"/>
+      <c r="BM66" s="1"/>
+      <c r="BN66" s="1"/>
+      <c r="BO66" s="1"/>
+      <c r="BP66" s="1"/>
+      <c r="BQ66" s="1"/>
+      <c r="BR66" s="1"/>
+      <c r="BS66" s="1"/>
+      <c r="BT66" s="1"/>
+    </row>
+    <row r="67" spans="1:72">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="1"/>
+      <c r="P67" s="1"/>
+      <c r="Q67" s="1"/>
+      <c r="R67" s="1"/>
+      <c r="S67" s="1"/>
+      <c r="T67" s="1"/>
+      <c r="U67" s="1"/>
+      <c r="V67" s="1"/>
+      <c r="W67" s="1"/>
+      <c r="X67" s="1"/>
+      <c r="Y67" s="1"/>
+      <c r="Z67" s="1"/>
+      <c r="AA67" s="1"/>
+      <c r="AB67" s="1"/>
+      <c r="AC67" s="1"/>
+      <c r="AD67" s="1"/>
+      <c r="AE67" s="1"/>
+      <c r="AF67" s="1"/>
+      <c r="AG67" s="1"/>
+      <c r="AH67" s="1"/>
+      <c r="AI67" s="1"/>
+      <c r="AJ67" s="1"/>
+      <c r="AK67" s="1"/>
+      <c r="AL67" s="1"/>
+      <c r="AM67" s="1"/>
+      <c r="AN67" s="1"/>
+      <c r="AO67" s="1"/>
+      <c r="AP67" s="1"/>
+      <c r="AQ67" s="1"/>
+      <c r="AR67" s="1"/>
+      <c r="AS67" s="1"/>
+      <c r="AT67" s="1"/>
+      <c r="AU67" s="1"/>
+      <c r="AV67" s="1"/>
+      <c r="AW67" s="1"/>
+      <c r="AX67" s="1"/>
+      <c r="AY67" s="1"/>
+      <c r="AZ67" s="1"/>
+      <c r="BA67" s="1"/>
+      <c r="BB67" s="1"/>
+      <c r="BC67" s="1"/>
+      <c r="BD67" s="1"/>
+      <c r="BE67" s="1"/>
+      <c r="BF67" s="1"/>
+      <c r="BG67" s="1"/>
+      <c r="BH67" s="1"/>
+      <c r="BI67" s="1"/>
+      <c r="BJ67" s="1"/>
+      <c r="BK67" s="1"/>
+      <c r="BL67" s="1"/>
+      <c r="BM67" s="1"/>
+      <c r="BN67" s="1"/>
+      <c r="BO67" s="1"/>
+      <c r="BP67" s="1"/>
+      <c r="BQ67" s="1"/>
+      <c r="BR67" s="1"/>
+      <c r="BS67" s="1"/>
+      <c r="BT67" s="1"/>
+    </row>
+    <row r="68" spans="1:72">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
+      <c r="P68" s="1"/>
+      <c r="Q68" s="1"/>
+      <c r="R68" s="1"/>
+      <c r="S68" s="1"/>
+      <c r="T68" s="1"/>
+      <c r="U68" s="1"/>
+      <c r="V68" s="1"/>
+      <c r="W68" s="1"/>
+      <c r="X68" s="1"/>
+      <c r="Y68" s="1"/>
+      <c r="Z68" s="1"/>
+      <c r="AA68" s="1"/>
+      <c r="AB68" s="1"/>
+      <c r="AC68" s="1"/>
+      <c r="AD68" s="1"/>
+      <c r="AE68" s="1"/>
+      <c r="AF68" s="1"/>
+      <c r="AG68" s="1"/>
+      <c r="AH68" s="1"/>
+      <c r="AI68" s="1"/>
+      <c r="AJ68" s="1"/>
+      <c r="AK68" s="1"/>
+      <c r="AL68" s="1"/>
+      <c r="AM68" s="1"/>
+      <c r="AN68" s="1"/>
+      <c r="AO68" s="1"/>
+      <c r="AP68" s="1"/>
+      <c r="AQ68" s="1"/>
+      <c r="AR68" s="1"/>
+      <c r="AS68" s="1"/>
+      <c r="AT68" s="1"/>
+      <c r="AU68" s="1"/>
+      <c r="AV68" s="1"/>
+      <c r="AW68" s="1"/>
+      <c r="AX68" s="1"/>
+      <c r="AY68" s="1"/>
+      <c r="AZ68" s="1"/>
+      <c r="BA68" s="1"/>
+      <c r="BB68" s="1"/>
+      <c r="BC68" s="1"/>
+      <c r="BD68" s="1"/>
+      <c r="BE68" s="1"/>
+      <c r="BF68" s="1"/>
+      <c r="BG68" s="1"/>
+      <c r="BH68" s="1"/>
+      <c r="BI68" s="1"/>
+      <c r="BJ68" s="1"/>
+      <c r="BK68" s="1"/>
+      <c r="BL68" s="1"/>
+      <c r="BM68" s="1"/>
+      <c r="BN68" s="1"/>
+      <c r="BO68" s="1"/>
+      <c r="BP68" s="1"/>
+      <c r="BQ68" s="1"/>
+      <c r="BR68" s="1"/>
+      <c r="BS68" s="1"/>
+      <c r="BT68" s="1"/>
+    </row>
+    <row r="69" spans="1:72">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
+      <c r="L69" s="1"/>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
+      <c r="O69" s="1"/>
+      <c r="P69" s="1"/>
+      <c r="Q69" s="1"/>
+      <c r="R69" s="1"/>
+      <c r="S69" s="1"/>
+      <c r="T69" s="1"/>
+      <c r="U69" s="1"/>
+      <c r="V69" s="1"/>
+      <c r="W69" s="1"/>
+      <c r="X69" s="1"/>
+      <c r="Y69" s="1"/>
+      <c r="Z69" s="1"/>
+      <c r="AA69" s="1"/>
+      <c r="AB69" s="1"/>
+      <c r="AC69" s="1"/>
+      <c r="AD69" s="1"/>
+      <c r="AE69" s="1"/>
+      <c r="AF69" s="1"/>
+      <c r="AG69" s="1"/>
+      <c r="AH69" s="1"/>
+      <c r="AI69" s="1"/>
+      <c r="AJ69" s="1"/>
+      <c r="AK69" s="1"/>
+      <c r="AL69" s="1"/>
+      <c r="AM69" s="1"/>
+      <c r="AN69" s="1"/>
+      <c r="AO69" s="1"/>
+      <c r="AP69" s="1"/>
+      <c r="AQ69" s="1"/>
+      <c r="AR69" s="1"/>
+      <c r="AS69" s="1"/>
+      <c r="AT69" s="1"/>
+      <c r="AU69" s="1"/>
+      <c r="AV69" s="1"/>
+      <c r="AW69" s="1"/>
+      <c r="AX69" s="1"/>
+      <c r="AY69" s="1"/>
+      <c r="AZ69" s="1"/>
+      <c r="BA69" s="1"/>
+      <c r="BB69" s="1"/>
+      <c r="BC69" s="1"/>
+      <c r="BD69" s="1"/>
+      <c r="BE69" s="1"/>
+      <c r="BF69" s="1"/>
+      <c r="BG69" s="1"/>
+      <c r="BH69" s="1"/>
+      <c r="BI69" s="1"/>
+      <c r="BJ69" s="1"/>
+      <c r="BK69" s="1"/>
+      <c r="BL69" s="1"/>
+      <c r="BM69" s="1"/>
+      <c r="BN69" s="1"/>
+      <c r="BO69" s="1"/>
+      <c r="BP69" s="1"/>
+      <c r="BQ69" s="1"/>
+      <c r="BR69" s="1"/>
+      <c r="BS69" s="1"/>
+      <c r="BT69" s="1"/>
+    </row>
+    <row r="70" spans="1:72">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
+      <c r="L70" s="1"/>
+      <c r="M70" s="1"/>
+      <c r="N70" s="1"/>
+      <c r="O70" s="1"/>
+      <c r="P70" s="1"/>
+      <c r="Q70" s="1"/>
+      <c r="R70" s="1"/>
+      <c r="S70" s="1"/>
+      <c r="T70" s="1"/>
+      <c r="U70" s="1"/>
+      <c r="V70" s="1"/>
+      <c r="W70" s="1"/>
+      <c r="X70" s="1"/>
+      <c r="Y70" s="1"/>
+      <c r="Z70" s="1"/>
+      <c r="AA70" s="1"/>
+      <c r="AB70" s="1"/>
+      <c r="AC70" s="1"/>
+      <c r="AD70" s="1"/>
+      <c r="AE70" s="1"/>
+      <c r="AF70" s="1"/>
+      <c r="AG70" s="1"/>
+      <c r="AH70" s="1"/>
+      <c r="AI70" s="1"/>
+      <c r="AJ70" s="1"/>
+      <c r="AK70" s="1"/>
+      <c r="AL70" s="1"/>
+      <c r="AM70" s="1"/>
+      <c r="AN70" s="1"/>
+      <c r="AO70" s="1"/>
+      <c r="AP70" s="1"/>
+      <c r="AQ70" s="1"/>
+      <c r="AR70" s="1"/>
+      <c r="AS70" s="1"/>
+      <c r="AT70" s="1"/>
+      <c r="AU70" s="1"/>
+      <c r="AV70" s="1"/>
+      <c r="AW70" s="1"/>
+      <c r="AX70" s="1"/>
+      <c r="AY70" s="1"/>
+      <c r="AZ70" s="1"/>
+      <c r="BA70" s="1"/>
+      <c r="BB70" s="1"/>
+      <c r="BC70" s="1"/>
+      <c r="BD70" s="1"/>
+      <c r="BE70" s="1"/>
+      <c r="BF70" s="1"/>
+      <c r="BG70" s="1"/>
+      <c r="BH70" s="1"/>
+      <c r="BI70" s="1"/>
+      <c r="BJ70" s="1"/>
+      <c r="BK70" s="1"/>
+      <c r="BL70" s="1"/>
+      <c r="BM70" s="1"/>
+      <c r="BN70" s="1"/>
+      <c r="BO70" s="1"/>
+      <c r="BP70" s="1"/>
+      <c r="BQ70" s="1"/>
+      <c r="BR70" s="1"/>
+      <c r="BS70" s="1"/>
+      <c r="BT70" s="1"/>
+    </row>
+    <row r="71" spans="1:72">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+      <c r="K71" s="1"/>
+      <c r="L71" s="1"/>
+      <c r="M71" s="1"/>
+      <c r="N71" s="1"/>
+      <c r="O71" s="1"/>
+      <c r="P71" s="1"/>
+      <c r="Q71" s="1"/>
+      <c r="R71" s="1"/>
+      <c r="S71" s="1"/>
+      <c r="T71" s="1"/>
+      <c r="U71" s="1"/>
+      <c r="V71" s="1"/>
+      <c r="W71" s="1"/>
+      <c r="X71" s="1"/>
+      <c r="Y71" s="1"/>
+      <c r="Z71" s="1"/>
+      <c r="AA71" s="1"/>
+      <c r="AB71" s="1"/>
+      <c r="AC71" s="1"/>
+      <c r="AD71" s="1"/>
+      <c r="AE71" s="1"/>
+      <c r="AF71" s="1"/>
+      <c r="AG71" s="1"/>
+      <c r="AH71" s="1"/>
+      <c r="AI71" s="1"/>
+      <c r="AJ71" s="1"/>
+      <c r="AK71" s="1"/>
+      <c r="AL71" s="1"/>
+      <c r="AM71" s="1"/>
+      <c r="AN71" s="1"/>
+      <c r="AO71" s="1"/>
+      <c r="AP71" s="1"/>
+      <c r="AQ71" s="1"/>
+      <c r="AR71" s="1"/>
+      <c r="AS71" s="1"/>
+      <c r="AT71" s="1"/>
+      <c r="AU71" s="1"/>
+      <c r="AV71" s="1"/>
+      <c r="AW71" s="1"/>
+      <c r="AX71" s="1"/>
+      <c r="AY71" s="1"/>
+      <c r="AZ71" s="1"/>
+      <c r="BA71" s="1"/>
+      <c r="BB71" s="1"/>
+      <c r="BC71" s="1"/>
+      <c r="BD71" s="1"/>
+      <c r="BE71" s="1"/>
+      <c r="BF71" s="1"/>
+      <c r="BG71" s="1"/>
+      <c r="BH71" s="1"/>
+      <c r="BI71" s="1"/>
+      <c r="BJ71" s="1"/>
+      <c r="BK71" s="1"/>
+      <c r="BL71" s="1"/>
+      <c r="BM71" s="1"/>
+      <c r="BN71" s="1"/>
+      <c r="BO71" s="1"/>
+      <c r="BP71" s="1"/>
+      <c r="BQ71" s="1"/>
+      <c r="BR71" s="1"/>
+      <c r="BS71" s="1"/>
+      <c r="BT71" s="1"/>
+    </row>
+    <row r="72" spans="1:72">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+      <c r="J72" s="1"/>
+      <c r="K72" s="1"/>
+      <c r="L72" s="1"/>
+      <c r="M72" s="1"/>
+      <c r="N72" s="1"/>
+      <c r="O72" s="1"/>
+      <c r="P72" s="1"/>
+      <c r="Q72" s="1"/>
+      <c r="R72" s="1"/>
+      <c r="S72" s="1"/>
+      <c r="T72" s="1"/>
+      <c r="U72" s="1"/>
+      <c r="V72" s="1"/>
+      <c r="W72" s="1"/>
+      <c r="X72" s="1"/>
+      <c r="Y72" s="1"/>
+      <c r="Z72" s="1"/>
+      <c r="AA72" s="1"/>
+      <c r="AB72" s="1"/>
+      <c r="AC72" s="1"/>
+      <c r="AD72" s="1"/>
+      <c r="AE72" s="1"/>
+      <c r="AF72" s="1"/>
+      <c r="AG72" s="1"/>
+      <c r="AH72" s="1"/>
+      <c r="AI72" s="1"/>
+      <c r="AJ72" s="1"/>
+      <c r="AK72" s="1"/>
+      <c r="AL72" s="1"/>
+      <c r="AM72" s="1"/>
+      <c r="AN72" s="1"/>
+      <c r="AO72" s="1"/>
+      <c r="AP72" s="1"/>
+      <c r="AQ72" s="1"/>
+      <c r="AR72" s="1"/>
+      <c r="AS72" s="1"/>
+      <c r="AT72" s="1"/>
+      <c r="AU72" s="1"/>
+      <c r="AV72" s="1"/>
+      <c r="AW72" s="1"/>
+      <c r="AX72" s="1"/>
+      <c r="AY72" s="1"/>
+      <c r="AZ72" s="1"/>
+      <c r="BA72" s="1"/>
+      <c r="BB72" s="1"/>
+      <c r="BC72" s="1"/>
+      <c r="BD72" s="1"/>
+      <c r="BE72" s="1"/>
+      <c r="BF72" s="1"/>
+      <c r="BG72" s="1"/>
+      <c r="BH72" s="1"/>
+      <c r="BI72" s="1"/>
+      <c r="BJ72" s="1"/>
+      <c r="BK72" s="1"/>
+      <c r="BL72" s="1"/>
+      <c r="BM72" s="1"/>
+      <c r="BN72" s="1"/>
+      <c r="BO72" s="1"/>
+      <c r="BP72" s="1"/>
+      <c r="BQ72" s="1"/>
+      <c r="BR72" s="1"/>
+      <c r="BS72" s="1"/>
+      <c r="BT72" s="1"/>
+    </row>
+    <row r="73" spans="1:72">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+      <c r="K73" s="1"/>
+      <c r="L73" s="1"/>
+      <c r="M73" s="1"/>
+      <c r="N73" s="1"/>
+      <c r="O73" s="1"/>
+      <c r="P73" s="1"/>
+      <c r="Q73" s="1"/>
+      <c r="R73" s="1"/>
+      <c r="S73" s="1"/>
+      <c r="T73" s="1"/>
+      <c r="U73" s="1"/>
+      <c r="V73" s="1"/>
+      <c r="W73" s="1"/>
+      <c r="X73" s="1"/>
+      <c r="Y73" s="1"/>
+      <c r="Z73" s="1"/>
+      <c r="AA73" s="1"/>
+      <c r="AB73" s="1"/>
+      <c r="AC73" s="1"/>
+      <c r="AD73" s="1"/>
+      <c r="AE73" s="1"/>
+      <c r="AF73" s="1"/>
+      <c r="AG73" s="1"/>
+      <c r="AH73" s="1"/>
+      <c r="AI73" s="1"/>
+      <c r="AJ73" s="1"/>
+      <c r="AK73" s="1"/>
+      <c r="AL73" s="1"/>
+      <c r="AM73" s="1"/>
+      <c r="AN73" s="1"/>
+      <c r="AO73" s="1"/>
+      <c r="AP73" s="1"/>
+      <c r="AQ73" s="1"/>
+      <c r="AR73" s="1"/>
+      <c r="AS73" s="1"/>
+      <c r="AT73" s="1"/>
+      <c r="AU73" s="1"/>
+      <c r="AV73" s="1"/>
+      <c r="AW73" s="1"/>
+      <c r="AX73" s="1"/>
+      <c r="AY73" s="1"/>
+      <c r="AZ73" s="1"/>
+      <c r="BA73" s="1"/>
+      <c r="BB73" s="1"/>
+      <c r="BC73" s="1"/>
+      <c r="BD73" s="1"/>
+      <c r="BE73" s="1"/>
+      <c r="BF73" s="1"/>
+      <c r="BG73" s="1"/>
+      <c r="BH73" s="1"/>
+      <c r="BI73" s="1"/>
+      <c r="BJ73" s="1"/>
+      <c r="BK73" s="1"/>
+      <c r="BL73" s="1"/>
+      <c r="BM73" s="1"/>
+      <c r="BN73" s="1"/>
+      <c r="BO73" s="1"/>
+      <c r="BP73" s="1"/>
+      <c r="BQ73" s="1"/>
+      <c r="BR73" s="1"/>
+      <c r="BS73" s="1"/>
+      <c r="BT73" s="1"/>
+    </row>
+    <row r="74" spans="1:72">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
+      <c r="K74" s="1"/>
+      <c r="L74" s="1"/>
+      <c r="M74" s="1"/>
+      <c r="N74" s="1"/>
+      <c r="O74" s="1"/>
+      <c r="P74" s="1"/>
+      <c r="Q74" s="1"/>
+      <c r="R74" s="1"/>
+      <c r="S74" s="1"/>
+      <c r="T74" s="1"/>
+      <c r="U74" s="1"/>
+      <c r="V74" s="1"/>
+      <c r="W74" s="1"/>
+      <c r="X74" s="1"/>
+      <c r="Y74" s="1"/>
+      <c r="Z74" s="1"/>
+      <c r="AA74" s="1"/>
+      <c r="AB74" s="1"/>
+      <c r="AC74" s="1"/>
+      <c r="AD74" s="1"/>
+      <c r="AE74" s="1"/>
+      <c r="AF74" s="1"/>
+      <c r="AG74" s="1"/>
+      <c r="AH74" s="1"/>
+      <c r="AI74" s="1"/>
+      <c r="AJ74" s="1"/>
+      <c r="AK74" s="1"/>
+      <c r="AL74" s="1"/>
+      <c r="AM74" s="1"/>
+      <c r="AN74" s="1"/>
+      <c r="AO74" s="1"/>
+      <c r="AP74" s="1"/>
+      <c r="AQ74" s="1"/>
+      <c r="AR74" s="1"/>
+      <c r="AS74" s="1"/>
+      <c r="AT74" s="1"/>
+      <c r="AU74" s="1"/>
+      <c r="AV74" s="1"/>
+      <c r="AW74" s="1"/>
+      <c r="AX74" s="1"/>
+      <c r="AY74" s="1"/>
+      <c r="AZ74" s="1"/>
+      <c r="BA74" s="1"/>
+      <c r="BB74" s="1"/>
+      <c r="BC74" s="1"/>
+      <c r="BD74" s="1"/>
+      <c r="BE74" s="1"/>
+      <c r="BF74" s="1"/>
+      <c r="BG74" s="1"/>
+      <c r="BH74" s="1"/>
+      <c r="BI74" s="1"/>
+      <c r="BJ74" s="1"/>
+      <c r="BK74" s="1"/>
+      <c r="BL74" s="1"/>
+      <c r="BM74" s="1"/>
+      <c r="BN74" s="1"/>
+      <c r="BO74" s="1"/>
+      <c r="BP74" s="1"/>
+      <c r="BQ74" s="1"/>
+      <c r="BR74" s="1"/>
+      <c r="BS74" s="1"/>
+      <c r="BT74" s="1"/>
+    </row>
+    <row r="75" spans="1:72">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+      <c r="J75" s="1"/>
+      <c r="K75" s="1"/>
+      <c r="L75" s="1"/>
+      <c r="M75" s="1"/>
+      <c r="N75" s="1"/>
+      <c r="O75" s="1"/>
+      <c r="P75" s="1"/>
+      <c r="Q75" s="1"/>
+      <c r="R75" s="1"/>
+      <c r="S75" s="1"/>
+      <c r="T75" s="1"/>
+      <c r="U75" s="1"/>
+      <c r="V75" s="1"/>
+      <c r="W75" s="1"/>
+      <c r="X75" s="1"/>
+      <c r="Y75" s="1"/>
+      <c r="Z75" s="1"/>
+      <c r="AA75" s="1"/>
+      <c r="AB75" s="1"/>
+      <c r="AC75" s="1"/>
+      <c r="AD75" s="1"/>
+      <c r="AE75" s="1"/>
+      <c r="AF75" s="1"/>
+      <c r="AG75" s="1"/>
+      <c r="AH75" s="1"/>
+      <c r="AI75" s="1"/>
+      <c r="AJ75" s="1"/>
+      <c r="AK75" s="1"/>
+      <c r="AL75" s="1"/>
+      <c r="AM75" s="1"/>
+      <c r="AN75" s="1"/>
+      <c r="AO75" s="1"/>
+      <c r="AP75" s="1"/>
+      <c r="AQ75" s="1"/>
+      <c r="AR75" s="1"/>
+      <c r="AS75" s="1"/>
+      <c r="AT75" s="1"/>
+      <c r="AU75" s="1"/>
+      <c r="AV75" s="1"/>
+      <c r="AW75" s="1"/>
+      <c r="AX75" s="1"/>
+      <c r="AY75" s="1"/>
+      <c r="AZ75" s="1"/>
+      <c r="BA75" s="1"/>
+      <c r="BB75" s="1"/>
+      <c r="BC75" s="1"/>
+      <c r="BD75" s="1"/>
+      <c r="BE75" s="1"/>
+      <c r="BF75" s="1"/>
+      <c r="BG75" s="1"/>
+      <c r="BH75" s="1"/>
+      <c r="BI75" s="1"/>
+      <c r="BJ75" s="1"/>
+      <c r="BK75" s="1"/>
+      <c r="BL75" s="1"/>
+      <c r="BM75" s="1"/>
+      <c r="BN75" s="1"/>
+      <c r="BO75" s="1"/>
+      <c r="BP75" s="1"/>
+      <c r="BQ75" s="1"/>
+      <c r="BR75" s="1"/>
+      <c r="BS75" s="1"/>
+      <c r="BT75" s="1"/>
+    </row>
+    <row r="76" spans="1:72">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
+      <c r="J76" s="1"/>
+      <c r="K76" s="1"/>
+      <c r="L76" s="1"/>
+      <c r="M76" s="1"/>
+      <c r="N76" s="1"/>
+      <c r="O76" s="1"/>
+      <c r="P76" s="1"/>
+      <c r="Q76" s="1"/>
+      <c r="R76" s="1"/>
+      <c r="S76" s="1"/>
+      <c r="T76" s="1"/>
+      <c r="U76" s="1"/>
+      <c r="V76" s="1"/>
+      <c r="W76" s="1"/>
+      <c r="X76" s="1"/>
+      <c r="Y76" s="1"/>
+      <c r="Z76" s="1"/>
+      <c r="AA76" s="1"/>
+      <c r="AB76" s="1"/>
+      <c r="AC76" s="1"/>
+      <c r="AD76" s="1"/>
+      <c r="AE76" s="1"/>
+      <c r="AF76" s="1"/>
+      <c r="AG76" s="1"/>
+      <c r="AH76" s="1"/>
+      <c r="AI76" s="1"/>
+      <c r="AJ76" s="1"/>
+      <c r="AK76" s="1"/>
+      <c r="AL76" s="1"/>
+      <c r="AM76" s="1"/>
+      <c r="AN76" s="1"/>
+      <c r="AO76" s="1"/>
+      <c r="AP76" s="1"/>
+      <c r="AQ76" s="1"/>
+      <c r="AR76" s="1"/>
+      <c r="AS76" s="1"/>
+      <c r="AT76" s="1"/>
+      <c r="AU76" s="1"/>
+      <c r="AV76" s="1"/>
+      <c r="AW76" s="1"/>
+      <c r="AX76" s="1"/>
+      <c r="AY76" s="1"/>
+      <c r="AZ76" s="1"/>
+      <c r="BA76" s="1"/>
+      <c r="BB76" s="1"/>
+      <c r="BC76" s="1"/>
+      <c r="BD76" s="1"/>
+      <c r="BE76" s="1"/>
+      <c r="BF76" s="1"/>
+      <c r="BG76" s="1"/>
+      <c r="BH76" s="1"/>
+      <c r="BI76" s="1"/>
+      <c r="BJ76" s="1"/>
+      <c r="BK76" s="1"/>
+      <c r="BL76" s="1"/>
+      <c r="BM76" s="1"/>
+      <c r="BN76" s="1"/>
+      <c r="BO76" s="1"/>
+      <c r="BP76" s="1"/>
+      <c r="BQ76" s="1"/>
+      <c r="BR76" s="1"/>
+      <c r="BS76" s="1"/>
+      <c r="BT76" s="1"/>
+    </row>
+    <row r="77" spans="1:72">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
+      <c r="K77" s="1"/>
+      <c r="L77" s="1"/>
+      <c r="M77" s="1"/>
+      <c r="N77" s="1"/>
+      <c r="O77" s="1"/>
+      <c r="P77" s="1"/>
+      <c r="Q77" s="1"/>
+      <c r="R77" s="1"/>
+      <c r="S77" s="1"/>
+      <c r="T77" s="1"/>
+      <c r="U77" s="1"/>
+      <c r="V77" s="1"/>
+      <c r="W77" s="1"/>
+      <c r="X77" s="1"/>
+      <c r="Y77" s="1"/>
+      <c r="Z77" s="1"/>
+      <c r="AA77" s="1"/>
+      <c r="AB77" s="1"/>
+      <c r="AC77" s="1"/>
+      <c r="AD77" s="1"/>
+      <c r="AE77" s="1"/>
+      <c r="AF77" s="1"/>
+      <c r="AG77" s="1"/>
+      <c r="AH77" s="1"/>
+      <c r="AI77" s="1"/>
+      <c r="AJ77" s="1"/>
+      <c r="AK77" s="1"/>
+      <c r="AL77" s="1"/>
+      <c r="AM77" s="1"/>
+      <c r="AN77" s="1"/>
+      <c r="AO77" s="1"/>
+      <c r="AP77" s="1"/>
+      <c r="AQ77" s="1"/>
+      <c r="AR77" s="1"/>
+      <c r="AS77" s="1"/>
+      <c r="AT77" s="1"/>
+      <c r="AU77" s="1"/>
+      <c r="AV77" s="1"/>
+      <c r="AW77" s="1"/>
+      <c r="AX77" s="1"/>
+      <c r="AY77" s="1"/>
+      <c r="AZ77" s="1"/>
+      <c r="BA77" s="1"/>
+      <c r="BB77" s="1"/>
+      <c r="BC77" s="1"/>
+      <c r="BD77" s="1"/>
+      <c r="BE77" s="1"/>
+      <c r="BF77" s="1"/>
+      <c r="BG77" s="1"/>
+      <c r="BH77" s="1"/>
+      <c r="BI77" s="1"/>
+      <c r="BJ77" s="1"/>
+      <c r="BK77" s="1"/>
+      <c r="BL77" s="1"/>
+      <c r="BM77" s="1"/>
+      <c r="BN77" s="1"/>
+      <c r="BO77" s="1"/>
+      <c r="BP77" s="1"/>
+      <c r="BQ77" s="1"/>
+      <c r="BR77" s="1"/>
+      <c r="BS77" s="1"/>
+      <c r="BT77" s="1"/>
+    </row>
+    <row r="78" spans="1:72">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
+      <c r="K78" s="1"/>
+      <c r="L78" s="1"/>
+      <c r="M78" s="1"/>
+      <c r="N78" s="1"/>
+      <c r="O78" s="1"/>
+      <c r="P78" s="1"/>
+      <c r="Q78" s="1"/>
+      <c r="R78" s="1"/>
+      <c r="S78" s="1"/>
+      <c r="T78" s="1"/>
+      <c r="U78" s="1"/>
+      <c r="V78" s="1"/>
+      <c r="W78" s="1"/>
+      <c r="X78" s="1"/>
+      <c r="Y78" s="1"/>
+      <c r="Z78" s="1"/>
+      <c r="AA78" s="1"/>
+      <c r="AB78" s="1"/>
+      <c r="AC78" s="1"/>
+      <c r="AD78" s="1"/>
+      <c r="AE78" s="1"/>
+      <c r="AF78" s="1"/>
+      <c r="AG78" s="1"/>
+      <c r="AH78" s="1"/>
+      <c r="AI78" s="1"/>
+      <c r="AJ78" s="1"/>
+      <c r="AK78" s="1"/>
+      <c r="AL78" s="1"/>
+      <c r="AM78" s="1"/>
+      <c r="AN78" s="1"/>
+      <c r="AO78" s="1"/>
+      <c r="AP78" s="1"/>
+      <c r="AQ78" s="1"/>
+      <c r="AR78" s="1"/>
+      <c r="AS78" s="1"/>
+      <c r="AT78" s="1"/>
+      <c r="AU78" s="1"/>
+      <c r="AV78" s="1"/>
+      <c r="AW78" s="1"/>
+      <c r="AX78" s="1"/>
+      <c r="AY78" s="1"/>
+      <c r="AZ78" s="1"/>
+      <c r="BA78" s="1"/>
+      <c r="BB78" s="1"/>
+      <c r="BC78" s="1"/>
+      <c r="BD78" s="1"/>
+      <c r="BE78" s="1"/>
+      <c r="BF78" s="1"/>
+      <c r="BG78" s="1"/>
+      <c r="BH78" s="1"/>
+      <c r="BI78" s="1"/>
+      <c r="BJ78" s="1"/>
+      <c r="BK78" s="1"/>
+      <c r="BL78" s="1"/>
+      <c r="BM78" s="1"/>
+      <c r="BN78" s="1"/>
+      <c r="BO78" s="1"/>
+      <c r="BP78" s="1"/>
+      <c r="BQ78" s="1"/>
+      <c r="BR78" s="1"/>
+      <c r="BS78" s="1"/>
+      <c r="BT78" s="1"/>
+    </row>
+    <row r="79" spans="1:72">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="1"/>
+      <c r="I79" s="1"/>
+      <c r="J79" s="1"/>
+      <c r="K79" s="1"/>
+      <c r="L79" s="1"/>
+      <c r="M79" s="1"/>
+      <c r="N79" s="1"/>
+      <c r="O79" s="1"/>
+      <c r="P79" s="1"/>
+      <c r="Q79" s="1"/>
+      <c r="R79" s="1"/>
+      <c r="S79" s="1"/>
+      <c r="T79" s="1"/>
+      <c r="U79" s="1"/>
+      <c r="V79" s="1"/>
+      <c r="W79" s="1"/>
+      <c r="X79" s="1"/>
+      <c r="Y79" s="1"/>
+      <c r="Z79" s="1"/>
+      <c r="AA79" s="1"/>
+      <c r="AB79" s="1"/>
+      <c r="AC79" s="1"/>
+      <c r="AD79" s="1"/>
+      <c r="AE79" s="1"/>
+      <c r="AF79" s="1"/>
+      <c r="AG79" s="1"/>
+      <c r="AH79" s="1"/>
+      <c r="AI79" s="1"/>
+      <c r="AJ79" s="1"/>
+      <c r="AK79" s="1"/>
+      <c r="AL79" s="1"/>
+      <c r="AM79" s="1"/>
+      <c r="AN79" s="1"/>
+      <c r="AO79" s="1"/>
+      <c r="AP79" s="1"/>
+      <c r="AQ79" s="1"/>
+      <c r="AR79" s="1"/>
+      <c r="AS79" s="1"/>
+      <c r="AT79" s="1"/>
+      <c r="AU79" s="1"/>
+      <c r="AV79" s="1"/>
+      <c r="AW79" s="1"/>
+      <c r="AX79" s="1"/>
+      <c r="AY79" s="1"/>
+      <c r="AZ79" s="1"/>
+      <c r="BA79" s="1"/>
+      <c r="BB79" s="1"/>
+      <c r="BC79" s="1"/>
+      <c r="BD79" s="1"/>
+      <c r="BE79" s="1"/>
+      <c r="BF79" s="1"/>
+      <c r="BG79" s="1"/>
+      <c r="BH79" s="1"/>
+      <c r="BI79" s="1"/>
+      <c r="BJ79" s="1"/>
+      <c r="BK79" s="1"/>
+      <c r="BL79" s="1"/>
+      <c r="BM79" s="1"/>
+      <c r="BN79" s="1"/>
+      <c r="BO79" s="1"/>
+      <c r="BP79" s="1"/>
+      <c r="BQ79" s="1"/>
+      <c r="BR79" s="1"/>
+      <c r="BS79" s="1"/>
+      <c r="BT79" s="1"/>
+    </row>
+    <row r="80" spans="1:72">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+      <c r="J80" s="1"/>
+      <c r="K80" s="1"/>
+      <c r="L80" s="1"/>
+      <c r="M80" s="1"/>
+      <c r="N80" s="1"/>
+      <c r="O80" s="1"/>
+      <c r="P80" s="1"/>
+      <c r="Q80" s="1"/>
+      <c r="R80" s="1"/>
+      <c r="S80" s="1"/>
+      <c r="T80" s="1"/>
+      <c r="U80" s="1"/>
+      <c r="V80" s="1"/>
+      <c r="W80" s="1"/>
+      <c r="X80" s="1"/>
+      <c r="Y80" s="1"/>
+      <c r="Z80" s="1"/>
+      <c r="AA80" s="1"/>
+      <c r="AB80" s="1"/>
+      <c r="AC80" s="1"/>
+      <c r="AD80" s="1"/>
+      <c r="AE80" s="1"/>
+      <c r="AF80" s="1"/>
+      <c r="AG80" s="1"/>
+      <c r="AH80" s="1"/>
+      <c r="AI80" s="1"/>
+      <c r="AJ80" s="1"/>
+      <c r="AK80" s="1"/>
+      <c r="AL80" s="1"/>
+      <c r="AM80" s="1"/>
+      <c r="AN80" s="1"/>
+      <c r="AO80" s="1"/>
+      <c r="AP80" s="1"/>
+      <c r="AQ80" s="1"/>
+      <c r="AR80" s="1"/>
+      <c r="AS80" s="1"/>
+      <c r="AT80" s="1"/>
+      <c r="AU80" s="1"/>
+      <c r="AV80" s="1"/>
+      <c r="AW80" s="1"/>
+      <c r="AX80" s="1"/>
+      <c r="AY80" s="1"/>
+      <c r="AZ80" s="1"/>
+      <c r="BA80" s="1"/>
+      <c r="BB80" s="1"/>
+      <c r="BC80" s="1"/>
+      <c r="BD80" s="1"/>
+      <c r="BE80" s="1"/>
+      <c r="BF80" s="1"/>
+      <c r="BG80" s="1"/>
+      <c r="BH80" s="1"/>
+      <c r="BI80" s="1"/>
+      <c r="BJ80" s="1"/>
+      <c r="BK80" s="1"/>
+      <c r="BL80" s="1"/>
+      <c r="BM80" s="1"/>
+      <c r="BN80" s="1"/>
+      <c r="BO80" s="1"/>
+      <c r="BP80" s="1"/>
+      <c r="BQ80" s="1"/>
+      <c r="BR80" s="1"/>
+      <c r="BS80" s="1"/>
+      <c r="BT80" s="1"/>
+    </row>
+    <row r="81" spans="1:72">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
+      <c r="J81" s="1"/>
+      <c r="K81" s="1"/>
+      <c r="L81" s="1"/>
+      <c r="M81" s="1"/>
+      <c r="N81" s="1"/>
+      <c r="O81" s="1"/>
+      <c r="P81" s="1"/>
+      <c r="Q81" s="1"/>
+      <c r="R81" s="1"/>
+      <c r="S81" s="1"/>
+      <c r="T81" s="1"/>
+      <c r="U81" s="1"/>
+      <c r="V81" s="1"/>
+      <c r="W81" s="1"/>
+      <c r="X81" s="1"/>
+      <c r="Y81" s="1"/>
+      <c r="Z81" s="1"/>
+      <c r="AA81" s="1"/>
+      <c r="AB81" s="1"/>
+      <c r="AC81" s="1"/>
+      <c r="AD81" s="1"/>
+      <c r="AE81" s="1"/>
+      <c r="AF81" s="1"/>
+      <c r="AG81" s="1"/>
+      <c r="AH81" s="1"/>
+      <c r="AI81" s="1"/>
+      <c r="AJ81" s="1"/>
+      <c r="AK81" s="1"/>
+      <c r="AL81" s="1"/>
+      <c r="AM81" s="1"/>
+      <c r="AN81" s="1"/>
+      <c r="AO81" s="1"/>
+      <c r="AP81" s="1"/>
+      <c r="AQ81" s="1"/>
+      <c r="AR81" s="1"/>
+      <c r="AS81" s="1"/>
+      <c r="AT81" s="1"/>
+      <c r="AU81" s="1"/>
+      <c r="AV81" s="1"/>
+      <c r="AW81" s="1"/>
+      <c r="AX81" s="1"/>
+      <c r="AY81" s="1"/>
+      <c r="AZ81" s="1"/>
+      <c r="BA81" s="1"/>
+      <c r="BB81" s="1"/>
+      <c r="BC81" s="1"/>
+      <c r="BD81" s="1"/>
+      <c r="BE81" s="1"/>
+      <c r="BF81" s="1"/>
+      <c r="BG81" s="1"/>
+      <c r="BH81" s="1"/>
+      <c r="BI81" s="1"/>
+      <c r="BJ81" s="1"/>
+      <c r="BK81" s="1"/>
+      <c r="BL81" s="1"/>
+      <c r="BM81" s="1"/>
+      <c r="BN81" s="1"/>
+      <c r="BO81" s="1"/>
+      <c r="BP81" s="1"/>
+      <c r="BQ81" s="1"/>
+      <c r="BR81" s="1"/>
+      <c r="BS81" s="1"/>
+      <c r="BT81" s="1"/>
+    </row>
+    <row r="82" spans="1:72">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+      <c r="J82" s="1"/>
+      <c r="K82" s="1"/>
+      <c r="L82" s="1"/>
+      <c r="M82" s="1"/>
+      <c r="N82" s="1"/>
+      <c r="O82" s="1"/>
+      <c r="P82" s="1"/>
+      <c r="Q82" s="1"/>
+      <c r="R82" s="1"/>
+      <c r="S82" s="1"/>
+      <c r="T82" s="1"/>
+      <c r="U82" s="1"/>
+      <c r="V82" s="1"/>
+      <c r="W82" s="1"/>
+      <c r="X82" s="1"/>
+      <c r="Y82" s="1"/>
+      <c r="Z82" s="1"/>
+      <c r="AA82" s="1"/>
+      <c r="AB82" s="1"/>
+      <c r="AC82" s="1"/>
+      <c r="AD82" s="1"/>
+      <c r="AE82" s="1"/>
+      <c r="AF82" s="1"/>
+      <c r="AG82" s="1"/>
+      <c r="AH82" s="1"/>
+      <c r="AI82" s="1"/>
+      <c r="AJ82" s="1"/>
+      <c r="AK82" s="1"/>
+      <c r="AL82" s="1"/>
+      <c r="AM82" s="1"/>
+      <c r="AN82" s="1"/>
+      <c r="AO82" s="1"/>
+      <c r="AP82" s="1"/>
+      <c r="AQ82" s="1"/>
+      <c r="AR82" s="1"/>
+      <c r="AS82" s="1"/>
+      <c r="AT82" s="1"/>
+      <c r="AU82" s="1"/>
+      <c r="AV82" s="1"/>
+      <c r="AW82" s="1"/>
+      <c r="AX82" s="1"/>
+      <c r="AY82" s="1"/>
+      <c r="AZ82" s="1"/>
+      <c r="BA82" s="1"/>
+      <c r="BB82" s="1"/>
+      <c r="BC82" s="1"/>
+      <c r="BD82" s="1"/>
+      <c r="BE82" s="1"/>
+      <c r="BF82" s="1"/>
+      <c r="BG82" s="1"/>
+      <c r="BH82" s="1"/>
+      <c r="BI82" s="1"/>
+      <c r="BJ82" s="1"/>
+      <c r="BK82" s="1"/>
+      <c r="BL82" s="1"/>
+      <c r="BM82" s="1"/>
+      <c r="BN82" s="1"/>
+      <c r="BO82" s="1"/>
+      <c r="BP82" s="1"/>
+      <c r="BQ82" s="1"/>
+      <c r="BR82" s="1"/>
+      <c r="BS82" s="1"/>
+      <c r="BT82" s="1"/>
+    </row>
+    <row r="83" spans="1:72">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+      <c r="I83" s="1"/>
+      <c r="J83" s="1"/>
+      <c r="K83" s="1"/>
+      <c r="L83" s="1"/>
+      <c r="M83" s="1"/>
+      <c r="N83" s="1"/>
+      <c r="O83" s="1"/>
+      <c r="P83" s="1"/>
+      <c r="Q83" s="1"/>
+      <c r="R83" s="1"/>
+      <c r="S83" s="1"/>
+      <c r="T83" s="1"/>
+      <c r="U83" s="1"/>
+      <c r="V83" s="1"/>
+      <c r="W83" s="1"/>
+      <c r="X83" s="1"/>
+      <c r="Y83" s="1"/>
+      <c r="Z83" s="1"/>
+      <c r="AA83" s="1"/>
+      <c r="AB83" s="1"/>
+      <c r="AC83" s="1"/>
+      <c r="AD83" s="1"/>
+      <c r="AE83" s="1"/>
+      <c r="AF83" s="1"/>
+      <c r="AG83" s="1"/>
+      <c r="AH83" s="1"/>
+      <c r="AI83" s="1"/>
+      <c r="AJ83" s="1"/>
+      <c r="AK83" s="1"/>
+      <c r="AL83" s="1"/>
+      <c r="AM83" s="1"/>
+      <c r="AN83" s="1"/>
+      <c r="AO83" s="1"/>
+      <c r="AP83" s="1"/>
+      <c r="AQ83" s="1"/>
+      <c r="AR83" s="1"/>
+      <c r="AS83" s="1"/>
+      <c r="AT83" s="1"/>
+      <c r="AU83" s="1"/>
+      <c r="AV83" s="1"/>
+      <c r="AW83" s="1"/>
+      <c r="AX83" s="1"/>
+      <c r="AY83" s="1"/>
+      <c r="AZ83" s="1"/>
+      <c r="BA83" s="1"/>
+      <c r="BB83" s="1"/>
+      <c r="BC83" s="1"/>
+      <c r="BD83" s="1"/>
+      <c r="BE83" s="1"/>
+      <c r="BF83" s="1"/>
+      <c r="BG83" s="1"/>
+      <c r="BH83" s="1"/>
+      <c r="BI83" s="1"/>
+      <c r="BJ83" s="1"/>
+      <c r="BK83" s="1"/>
+      <c r="BL83" s="1"/>
+      <c r="BM83" s="1"/>
+      <c r="BN83" s="1"/>
+      <c r="BO83" s="1"/>
+      <c r="BP83" s="1"/>
+      <c r="BQ83" s="1"/>
+      <c r="BR83" s="1"/>
+      <c r="BS83" s="1"/>
+      <c r="BT83" s="1"/>
+    </row>
+    <row r="84" spans="1:72">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+      <c r="I84" s="1"/>
+      <c r="J84" s="1"/>
+      <c r="K84" s="1"/>
+      <c r="L84" s="1"/>
+      <c r="M84" s="1"/>
+      <c r="N84" s="1"/>
+      <c r="O84" s="1"/>
+      <c r="P84" s="1"/>
+      <c r="Q84" s="1"/>
+      <c r="R84" s="1"/>
+      <c r="S84" s="1"/>
+      <c r="T84" s="1"/>
+      <c r="U84" s="1"/>
+      <c r="V84" s="1"/>
+      <c r="W84" s="1"/>
+      <c r="X84" s="1"/>
+      <c r="Y84" s="1"/>
+      <c r="Z84" s="1"/>
+      <c r="AA84" s="1"/>
+      <c r="AB84" s="1"/>
+      <c r="AC84" s="1"/>
+      <c r="AD84" s="1"/>
+      <c r="AE84" s="1"/>
+      <c r="AF84" s="1"/>
+      <c r="AG84" s="1"/>
+      <c r="AH84" s="1"/>
+      <c r="AI84" s="1"/>
+      <c r="AJ84" s="1"/>
+      <c r="AK84" s="1"/>
+      <c r="AL84" s="1"/>
+      <c r="AM84" s="1"/>
+      <c r="AN84" s="1"/>
+      <c r="AO84" s="1"/>
+      <c r="AP84" s="1"/>
+      <c r="AQ84" s="1"/>
+      <c r="AR84" s="1"/>
+      <c r="AS84" s="1"/>
+      <c r="AT84" s="1"/>
+      <c r="AU84" s="1"/>
+      <c r="AV84" s="1"/>
+      <c r="AW84" s="1"/>
+      <c r="AX84" s="1"/>
+      <c r="AY84" s="1"/>
+      <c r="AZ84" s="1"/>
+      <c r="BA84" s="1"/>
+      <c r="BB84" s="1"/>
+      <c r="BC84" s="1"/>
+      <c r="BD84" s="1"/>
+      <c r="BE84" s="1"/>
+      <c r="BF84" s="1"/>
+      <c r="BG84" s="1"/>
+      <c r="BH84" s="1"/>
+      <c r="BI84" s="1"/>
+      <c r="BJ84" s="1"/>
+      <c r="BK84" s="1"/>
+      <c r="BL84" s="1"/>
+      <c r="BM84" s="1"/>
+      <c r="BN84" s="1"/>
+      <c r="BO84" s="1"/>
+      <c r="BP84" s="1"/>
+      <c r="BQ84" s="1"/>
+      <c r="BR84" s="1"/>
+      <c r="BS84" s="1"/>
+      <c r="BT84" s="1"/>
+    </row>
+    <row r="85" spans="1:72">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+      <c r="I85" s="1"/>
+      <c r="J85" s="1"/>
+      <c r="K85" s="1"/>
+      <c r="L85" s="1"/>
+      <c r="M85" s="1"/>
+      <c r="N85" s="1"/>
+      <c r="O85" s="1"/>
+      <c r="P85" s="1"/>
+      <c r="Q85" s="1"/>
+      <c r="R85" s="1"/>
+      <c r="S85" s="1"/>
+      <c r="T85" s="1"/>
+      <c r="U85" s="1"/>
+      <c r="V85" s="1"/>
+      <c r="W85" s="1"/>
+      <c r="X85" s="1"/>
+      <c r="Y85" s="1"/>
+      <c r="Z85" s="1"/>
+      <c r="AA85" s="1"/>
+      <c r="AB85" s="1"/>
+      <c r="AC85" s="1"/>
+      <c r="AD85" s="1"/>
+      <c r="AE85" s="1"/>
+      <c r="AF85" s="1"/>
+      <c r="AG85" s="1"/>
+      <c r="AH85" s="1"/>
+      <c r="AI85" s="1"/>
+      <c r="AJ85" s="1"/>
+      <c r="AK85" s="1"/>
+      <c r="AL85" s="1"/>
+      <c r="AM85" s="1"/>
+      <c r="AN85" s="1"/>
+      <c r="AO85" s="1"/>
+      <c r="AP85" s="1"/>
+      <c r="AQ85" s="1"/>
+      <c r="AR85" s="1"/>
+      <c r="AS85" s="1"/>
+      <c r="AT85" s="1"/>
+      <c r="AU85" s="1"/>
+      <c r="AV85" s="1"/>
+      <c r="AW85" s="1"/>
+      <c r="AX85" s="1"/>
+      <c r="AY85" s="1"/>
+      <c r="AZ85" s="1"/>
+      <c r="BA85" s="1"/>
+      <c r="BB85" s="1"/>
+      <c r="BC85" s="1"/>
+      <c r="BD85" s="1"/>
+      <c r="BE85" s="1"/>
+      <c r="BF85" s="1"/>
+      <c r="BG85" s="1"/>
+      <c r="BH85" s="1"/>
+      <c r="BI85" s="1"/>
+      <c r="BJ85" s="1"/>
+      <c r="BK85" s="1"/>
+      <c r="BL85" s="1"/>
+      <c r="BM85" s="1"/>
+      <c r="BN85" s="1"/>
+      <c r="BO85" s="1"/>
+      <c r="BP85" s="1"/>
+      <c r="BQ85" s="1"/>
+      <c r="BR85" s="1"/>
+      <c r="BS85" s="1"/>
+      <c r="BT85" s="1"/>
+    </row>
+    <row r="86" spans="1:72">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+      <c r="I86" s="1"/>
+      <c r="J86" s="1"/>
+      <c r="K86" s="1"/>
+      <c r="L86" s="1"/>
+      <c r="M86" s="1"/>
+      <c r="N86" s="1"/>
+      <c r="O86" s="1"/>
+      <c r="P86" s="1"/>
+      <c r="Q86" s="1"/>
+      <c r="R86" s="1"/>
+      <c r="S86" s="1"/>
+      <c r="T86" s="1"/>
+      <c r="U86" s="1"/>
+      <c r="V86" s="1"/>
+      <c r="W86" s="1"/>
+      <c r="X86" s="1"/>
+      <c r="Y86" s="1"/>
+      <c r="Z86" s="1"/>
+      <c r="AA86" s="1"/>
+      <c r="AB86" s="1"/>
+      <c r="AC86" s="1"/>
+      <c r="AD86" s="1"/>
+      <c r="AE86" s="1"/>
+      <c r="AF86" s="1"/>
+      <c r="AG86" s="1"/>
+      <c r="AH86" s="1"/>
+      <c r="AI86" s="1"/>
+      <c r="AJ86" s="1"/>
+      <c r="AK86" s="1"/>
+      <c r="AL86" s="1"/>
+      <c r="AM86" s="1"/>
+      <c r="AN86" s="1"/>
+      <c r="AO86" s="1"/>
+      <c r="AP86" s="1"/>
+      <c r="AQ86" s="1"/>
+      <c r="AR86" s="1"/>
+      <c r="AS86" s="1"/>
+      <c r="AT86" s="1"/>
+      <c r="AU86" s="1"/>
+      <c r="AV86" s="1"/>
+      <c r="AW86" s="1"/>
+      <c r="AX86" s="1"/>
+      <c r="AY86" s="1"/>
+      <c r="AZ86" s="1"/>
+      <c r="BA86" s="1"/>
+      <c r="BB86" s="1"/>
+      <c r="BC86" s="1"/>
+      <c r="BD86" s="1"/>
+      <c r="BE86" s="1"/>
+      <c r="BF86" s="1"/>
+      <c r="BG86" s="1"/>
+      <c r="BH86" s="1"/>
+      <c r="BI86" s="1"/>
+      <c r="BJ86" s="1"/>
+      <c r="BK86" s="1"/>
+      <c r="BL86" s="1"/>
+      <c r="BM86" s="1"/>
+      <c r="BN86" s="1"/>
+      <c r="BO86" s="1"/>
+      <c r="BP86" s="1"/>
+      <c r="BQ86" s="1"/>
+      <c r="BR86" s="1"/>
+      <c r="BS86" s="1"/>
+      <c r="BT86" s="1"/>
+    </row>
+    <row r="87" spans="1:72">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+      <c r="I87" s="1"/>
+      <c r="J87" s="1"/>
+      <c r="K87" s="1"/>
+      <c r="L87" s="1"/>
+      <c r="M87" s="1"/>
+      <c r="N87" s="1"/>
+      <c r="O87" s="1"/>
+      <c r="P87" s="1"/>
+      <c r="Q87" s="1"/>
+      <c r="R87" s="1"/>
+      <c r="S87" s="1"/>
+      <c r="T87" s="1"/>
+      <c r="U87" s="1"/>
+      <c r="V87" s="1"/>
+      <c r="W87" s="1"/>
+      <c r="X87" s="1"/>
+      <c r="Y87" s="1"/>
+      <c r="Z87" s="1"/>
+      <c r="AA87" s="1"/>
+      <c r="AB87" s="1"/>
+      <c r="AC87" s="1"/>
+      <c r="AD87" s="1"/>
+      <c r="AE87" s="1"/>
+      <c r="AF87" s="1"/>
+      <c r="AG87" s="1"/>
+      <c r="AH87" s="1"/>
+      <c r="AI87" s="1"/>
+      <c r="AJ87" s="1"/>
+      <c r="AK87" s="1"/>
+      <c r="AL87" s="1"/>
+      <c r="AM87" s="1"/>
+      <c r="AN87" s="1"/>
+      <c r="AO87" s="1"/>
+      <c r="AP87" s="1"/>
+      <c r="AQ87" s="1"/>
+      <c r="AR87" s="1"/>
+      <c r="AS87" s="1"/>
+      <c r="AT87" s="1"/>
+      <c r="AU87" s="1"/>
+      <c r="AV87" s="1"/>
+      <c r="AW87" s="1"/>
+      <c r="AX87" s="1"/>
+      <c r="AY87" s="1"/>
+      <c r="AZ87" s="1"/>
+      <c r="BA87" s="1"/>
+      <c r="BB87" s="1"/>
+      <c r="BC87" s="1"/>
+      <c r="BD87" s="1"/>
+      <c r="BE87" s="1"/>
+      <c r="BF87" s="1"/>
+      <c r="BG87" s="1"/>
+      <c r="BH87" s="1"/>
+      <c r="BI87" s="1"/>
+      <c r="BJ87" s="1"/>
+      <c r="BK87" s="1"/>
+      <c r="BL87" s="1"/>
+      <c r="BM87" s="1"/>
+      <c r="BN87" s="1"/>
+      <c r="BO87" s="1"/>
+      <c r="BP87" s="1"/>
+      <c r="BQ87" s="1"/>
+      <c r="BR87" s="1"/>
+      <c r="BS87" s="1"/>
+      <c r="BT87" s="1"/>
+    </row>
+    <row r="88" spans="1:72">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1"/>
+      <c r="F88" s="1"/>
+      <c r="G88" s="1"/>
+      <c r="H88" s="1"/>
+      <c r="I88" s="1"/>
+      <c r="J88" s="1"/>
+      <c r="K88" s="1"/>
+      <c r="L88" s="1"/>
+      <c r="M88" s="1"/>
+      <c r="N88" s="1"/>
+      <c r="O88" s="1"/>
+      <c r="P88" s="1"/>
+      <c r="Q88" s="1"/>
+      <c r="R88" s="1"/>
+      <c r="S88" s="1"/>
+      <c r="T88" s="1"/>
+      <c r="U88" s="1"/>
+      <c r="V88" s="1"/>
+      <c r="W88" s="1"/>
+      <c r="X88" s="1"/>
+      <c r="Y88" s="1"/>
+      <c r="Z88" s="1"/>
+      <c r="AA88" s="1"/>
+      <c r="AB88" s="1"/>
+      <c r="AC88" s="1"/>
+      <c r="AD88" s="1"/>
+      <c r="AE88" s="1"/>
+      <c r="AF88" s="1"/>
+      <c r="AG88" s="1"/>
+      <c r="AH88" s="1"/>
+      <c r="AI88" s="1"/>
+      <c r="AJ88" s="1"/>
+      <c r="AK88" s="1"/>
+      <c r="AL88" s="1"/>
+      <c r="AM88" s="1"/>
+      <c r="AN88" s="1"/>
+      <c r="AO88" s="1"/>
+      <c r="AP88" s="1"/>
+      <c r="AQ88" s="1"/>
+      <c r="AR88" s="1"/>
+      <c r="AS88" s="1"/>
+      <c r="AT88" s="1"/>
+      <c r="AU88" s="1"/>
+      <c r="AV88" s="1"/>
+      <c r="AW88" s="1"/>
+      <c r="AX88" s="1"/>
+      <c r="AY88" s="1"/>
+      <c r="AZ88" s="1"/>
+      <c r="BA88" s="1"/>
+      <c r="BB88" s="1"/>
+      <c r="BC88" s="1"/>
+      <c r="BD88" s="1"/>
+      <c r="BE88" s="1"/>
+      <c r="BF88" s="1"/>
+      <c r="BG88" s="1"/>
+      <c r="BH88" s="1"/>
+      <c r="BI88" s="1"/>
+      <c r="BJ88" s="1"/>
+      <c r="BK88" s="1"/>
+      <c r="BL88" s="1"/>
+      <c r="BM88" s="1"/>
+      <c r="BN88" s="1"/>
+      <c r="BO88" s="1"/>
+      <c r="BP88" s="1"/>
+      <c r="BQ88" s="1"/>
+      <c r="BR88" s="1"/>
+      <c r="BS88" s="1"/>
+      <c r="BT88" s="1"/>
+    </row>
+    <row r="89" spans="1:72">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1"/>
+      <c r="G89" s="1"/>
+      <c r="H89" s="1"/>
+      <c r="I89" s="1"/>
+      <c r="J89" s="1"/>
+      <c r="K89" s="1"/>
+      <c r="L89" s="1"/>
+      <c r="M89" s="1"/>
+      <c r="N89" s="1"/>
+      <c r="O89" s="1"/>
+      <c r="P89" s="1"/>
+      <c r="Q89" s="1"/>
+      <c r="R89" s="1"/>
+      <c r="S89" s="1"/>
+      <c r="T89" s="1"/>
+      <c r="U89" s="1"/>
+      <c r="V89" s="1"/>
+      <c r="W89" s="1"/>
+      <c r="X89" s="1"/>
+      <c r="Y89" s="1"/>
+      <c r="Z89" s="1"/>
+      <c r="AA89" s="1"/>
+      <c r="AB89" s="1"/>
+      <c r="AC89" s="1"/>
+      <c r="AD89" s="1"/>
+      <c r="AE89" s="1"/>
+      <c r="AF89" s="1"/>
+      <c r="AG89" s="1"/>
+      <c r="AH89" s="1"/>
+      <c r="AI89" s="1"/>
+      <c r="AJ89" s="1"/>
+      <c r="AK89" s="1"/>
+      <c r="AL89" s="1"/>
+      <c r="AM89" s="1"/>
+      <c r="AN89" s="1"/>
+      <c r="AO89" s="1"/>
+      <c r="AP89" s="1"/>
+      <c r="AQ89" s="1"/>
+      <c r="AR89" s="1"/>
+      <c r="AS89" s="1"/>
+      <c r="AT89" s="1"/>
+      <c r="AU89" s="1"/>
+      <c r="AV89" s="1"/>
+      <c r="AW89" s="1"/>
+      <c r="AX89" s="1"/>
+      <c r="AY89" s="1"/>
+      <c r="AZ89" s="1"/>
+      <c r="BA89" s="1"/>
+      <c r="BB89" s="1"/>
+      <c r="BC89" s="1"/>
+      <c r="BD89" s="1"/>
+      <c r="BE89" s="1"/>
+      <c r="BF89" s="1"/>
+      <c r="BG89" s="1"/>
+      <c r="BH89" s="1"/>
+      <c r="BI89" s="1"/>
+      <c r="BJ89" s="1"/>
+      <c r="BK89" s="1"/>
+      <c r="BL89" s="1"/>
+      <c r="BM89" s="1"/>
+      <c r="BN89" s="1"/>
+      <c r="BO89" s="1"/>
+      <c r="BP89" s="1"/>
+      <c r="BQ89" s="1"/>
+      <c r="BR89" s="1"/>
+      <c r="BS89" s="1"/>
+      <c r="BT89" s="1"/>
+    </row>
+    <row r="90" spans="1:72">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1"/>
+      <c r="F90" s="1"/>
+      <c r="G90" s="1"/>
+      <c r="H90" s="1"/>
+      <c r="I90" s="1"/>
+      <c r="J90" s="1"/>
+      <c r="K90" s="1"/>
+      <c r="L90" s="1"/>
+      <c r="M90" s="1"/>
+      <c r="N90" s="1"/>
+      <c r="O90" s="1"/>
+      <c r="P90" s="1"/>
+      <c r="Q90" s="1"/>
+      <c r="R90" s="1"/>
+      <c r="S90" s="1"/>
+      <c r="T90" s="1"/>
+      <c r="U90" s="1"/>
+      <c r="V90" s="1"/>
+      <c r="W90" s="1"/>
+      <c r="X90" s="1"/>
+      <c r="Y90" s="1"/>
+      <c r="Z90" s="1"/>
+      <c r="AA90" s="1"/>
+      <c r="AB90" s="1"/>
+      <c r="AC90" s="1"/>
+      <c r="AD90" s="1"/>
+      <c r="AE90" s="1"/>
+      <c r="AF90" s="1"/>
+      <c r="AG90" s="1"/>
+      <c r="AH90" s="1"/>
+      <c r="AI90" s="1"/>
+      <c r="AJ90" s="1"/>
+      <c r="AK90" s="1"/>
+      <c r="AL90" s="1"/>
+      <c r="AM90" s="1"/>
+      <c r="AN90" s="1"/>
+      <c r="AO90" s="1"/>
+      <c r="AP90" s="1"/>
+      <c r="AQ90" s="1"/>
+      <c r="AR90" s="1"/>
+      <c r="AS90" s="1"/>
+      <c r="AT90" s="1"/>
+      <c r="AU90" s="1"/>
+      <c r="AV90" s="1"/>
+      <c r="AW90" s="1"/>
+      <c r="AX90" s="1"/>
+      <c r="AY90" s="1"/>
+      <c r="AZ90" s="1"/>
+      <c r="BA90" s="1"/>
+      <c r="BB90" s="1"/>
+      <c r="BC90" s="1"/>
+      <c r="BD90" s="1"/>
+      <c r="BE90" s="1"/>
+      <c r="BF90" s="1"/>
+      <c r="BG90" s="1"/>
+      <c r="BH90" s="1"/>
+      <c r="BI90" s="1"/>
+      <c r="BJ90" s="1"/>
+      <c r="BK90" s="1"/>
+      <c r="BL90" s="1"/>
+      <c r="BM90" s="1"/>
+      <c r="BN90" s="1"/>
+      <c r="BO90" s="1"/>
+      <c r="BP90" s="1"/>
+      <c r="BQ90" s="1"/>
+      <c r="BR90" s="1"/>
+      <c r="BS90" s="1"/>
+      <c r="BT90" s="1"/>
+    </row>
+    <row r="91" spans="1:72">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
+      <c r="H91" s="1"/>
+      <c r="I91" s="1"/>
+      <c r="J91" s="1"/>
+      <c r="K91" s="1"/>
+      <c r="L91" s="1"/>
+      <c r="M91" s="1"/>
+      <c r="N91" s="1"/>
+      <c r="O91" s="1"/>
+      <c r="P91" s="1"/>
+      <c r="Q91" s="1"/>
+      <c r="R91" s="1"/>
+      <c r="S91" s="1"/>
+      <c r="T91" s="1"/>
+      <c r="U91" s="1"/>
+      <c r="V91" s="1"/>
+      <c r="W91" s="1"/>
+      <c r="X91" s="1"/>
+      <c r="Y91" s="1"/>
+      <c r="Z91" s="1"/>
+      <c r="AA91" s="1"/>
+      <c r="AB91" s="1"/>
+      <c r="AC91" s="1"/>
+      <c r="AD91" s="1"/>
+      <c r="AE91" s="1"/>
+      <c r="AF91" s="1"/>
+      <c r="AG91" s="1"/>
+      <c r="AH91" s="1"/>
+      <c r="AI91" s="1"/>
+      <c r="AJ91" s="1"/>
+      <c r="AK91" s="1"/>
+      <c r="AL91" s="1"/>
+      <c r="AM91" s="1"/>
+      <c r="AN91" s="1"/>
+      <c r="AO91" s="1"/>
+      <c r="AP91" s="1"/>
+      <c r="AQ91" s="1"/>
+      <c r="AR91" s="1"/>
+      <c r="AS91" s="1"/>
+      <c r="AT91" s="1"/>
+      <c r="AU91" s="1"/>
+      <c r="AV91" s="1"/>
+      <c r="AW91" s="1"/>
+      <c r="AX91" s="1"/>
+      <c r="AY91" s="1"/>
+      <c r="AZ91" s="1"/>
+      <c r="BA91" s="1"/>
+      <c r="BB91" s="1"/>
+      <c r="BC91" s="1"/>
+      <c r="BD91" s="1"/>
+      <c r="BE91" s="1"/>
+      <c r="BF91" s="1"/>
+      <c r="BG91" s="1"/>
+      <c r="BH91" s="1"/>
+      <c r="BI91" s="1"/>
+      <c r="BJ91" s="1"/>
+      <c r="BK91" s="1"/>
+      <c r="BL91" s="1"/>
+      <c r="BM91" s="1"/>
+      <c r="BN91" s="1"/>
+      <c r="BO91" s="1"/>
+      <c r="BP91" s="1"/>
+      <c r="BQ91" s="1"/>
+      <c r="BR91" s="1"/>
+      <c r="BS91" s="1"/>
+      <c r="BT91" s="1"/>
+    </row>
+    <row r="92" spans="1:72">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
+      <c r="H92" s="1"/>
+      <c r="I92" s="1"/>
+      <c r="J92" s="1"/>
+      <c r="K92" s="1"/>
+      <c r="L92" s="1"/>
+      <c r="M92" s="1"/>
+      <c r="N92" s="1"/>
+      <c r="O92" s="1"/>
+      <c r="P92" s="1"/>
+      <c r="Q92" s="1"/>
+      <c r="R92" s="1"/>
+      <c r="S92" s="1"/>
+      <c r="T92" s="1"/>
+      <c r="U92" s="1"/>
+      <c r="V92" s="1"/>
+      <c r="W92" s="1"/>
+      <c r="X92" s="1"/>
+      <c r="Y92" s="1"/>
+      <c r="Z92" s="1"/>
+      <c r="AA92" s="1"/>
+      <c r="AB92" s="1"/>
+      <c r="AC92" s="1"/>
+      <c r="AD92" s="1"/>
+      <c r="AE92" s="1"/>
+      <c r="AF92" s="1"/>
+      <c r="AG92" s="1"/>
+      <c r="AH92" s="1"/>
+      <c r="AI92" s="1"/>
+      <c r="AJ92" s="1"/>
+      <c r="AK92" s="1"/>
+      <c r="AL92" s="1"/>
+      <c r="AM92" s="1"/>
+      <c r="AN92" s="1"/>
+      <c r="AO92" s="1"/>
+      <c r="AP92" s="1"/>
+      <c r="AQ92" s="1"/>
+      <c r="AR92" s="1"/>
+      <c r="AS92" s="1"/>
+      <c r="AT92" s="1"/>
+      <c r="AU92" s="1"/>
+      <c r="AV92" s="1"/>
+      <c r="AW92" s="1"/>
+      <c r="AX92" s="1"/>
+      <c r="AY92" s="1"/>
+      <c r="AZ92" s="1"/>
+      <c r="BA92" s="1"/>
+      <c r="BB92" s="1"/>
+      <c r="BC92" s="1"/>
+      <c r="BD92" s="1"/>
+      <c r="BE92" s="1"/>
+      <c r="BF92" s="1"/>
+      <c r="BG92" s="1"/>
+      <c r="BH92" s="1"/>
+      <c r="BI92" s="1"/>
+      <c r="BJ92" s="1"/>
+      <c r="BK92" s="1"/>
+      <c r="BL92" s="1"/>
+      <c r="BM92" s="1"/>
+      <c r="BN92" s="1"/>
+      <c r="BO92" s="1"/>
+      <c r="BP92" s="1"/>
+      <c r="BQ92" s="1"/>
+      <c r="BR92" s="1"/>
+      <c r="BS92" s="1"/>
+      <c r="BT92" s="1"/>
+    </row>
+    <row r="93" spans="1:72">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+      <c r="H93" s="1"/>
+      <c r="I93" s="1"/>
+      <c r="J93" s="1"/>
+      <c r="K93" s="1"/>
+      <c r="L93" s="1"/>
+      <c r="M93" s="1"/>
+      <c r="N93" s="1"/>
+      <c r="O93" s="1"/>
+      <c r="P93" s="1"/>
+      <c r="Q93" s="1"/>
+      <c r="R93" s="1"/>
+      <c r="S93" s="1"/>
+      <c r="T93" s="1"/>
+      <c r="U93" s="1"/>
+      <c r="V93" s="1"/>
+      <c r="W93" s="1"/>
+      <c r="X93" s="1"/>
+      <c r="Y93" s="1"/>
+      <c r="Z93" s="1"/>
+      <c r="AA93" s="1"/>
+      <c r="AB93" s="1"/>
+      <c r="AC93" s="1"/>
+      <c r="AD93" s="1"/>
+      <c r="AE93" s="1"/>
+      <c r="AF93" s="1"/>
+      <c r="AG93" s="1"/>
+      <c r="AH93" s="1"/>
+      <c r="AI93" s="1"/>
+      <c r="AJ93" s="1"/>
+      <c r="AK93" s="1"/>
+      <c r="AL93" s="1"/>
+      <c r="AM93" s="1"/>
+      <c r="AN93" s="1"/>
+      <c r="AO93" s="1"/>
+      <c r="AP93" s="1"/>
+      <c r="AQ93" s="1"/>
+      <c r="AR93" s="1"/>
+      <c r="AS93" s="1"/>
+      <c r="AT93" s="1"/>
+      <c r="AU93" s="1"/>
+      <c r="AV93" s="1"/>
+      <c r="AW93" s="1"/>
+      <c r="AX93" s="1"/>
+      <c r="AY93" s="1"/>
+      <c r="AZ93" s="1"/>
+      <c r="BA93" s="1"/>
+      <c r="BB93" s="1"/>
+      <c r="BC93" s="1"/>
+      <c r="BD93" s="1"/>
+      <c r="BE93" s="1"/>
+      <c r="BF93" s="1"/>
+      <c r="BG93" s="1"/>
+      <c r="BH93" s="1"/>
+      <c r="BI93" s="1"/>
+      <c r="BJ93" s="1"/>
+      <c r="BK93" s="1"/>
+      <c r="BL93" s="1"/>
+      <c r="BM93" s="1"/>
+      <c r="BN93" s="1"/>
+      <c r="BO93" s="1"/>
+      <c r="BP93" s="1"/>
+      <c r="BQ93" s="1"/>
+      <c r="BR93" s="1"/>
+      <c r="BS93" s="1"/>
+      <c r="BT93" s="1"/>
+    </row>
+    <row r="94" spans="1:72">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="1"/>
+      <c r="I94" s="1"/>
+      <c r="J94" s="1"/>
+      <c r="K94" s="1"/>
+      <c r="L94" s="1"/>
+      <c r="M94" s="1"/>
+      <c r="N94" s="1"/>
+      <c r="O94" s="1"/>
+      <c r="P94" s="1"/>
+      <c r="Q94" s="1"/>
+      <c r="R94" s="1"/>
+      <c r="S94" s="1"/>
+      <c r="T94" s="1"/>
+      <c r="U94" s="1"/>
+      <c r="V94" s="1"/>
+      <c r="W94" s="1"/>
+      <c r="X94" s="1"/>
+      <c r="Y94" s="1"/>
+      <c r="Z94" s="1"/>
+      <c r="AA94" s="1"/>
+      <c r="AB94" s="1"/>
+      <c r="AC94" s="1"/>
+      <c r="AD94" s="1"/>
+      <c r="AE94" s="1"/>
+      <c r="AF94" s="1"/>
+      <c r="AG94" s="1"/>
+      <c r="AH94" s="1"/>
+      <c r="AI94" s="1"/>
+      <c r="AJ94" s="1"/>
+      <c r="AK94" s="1"/>
+      <c r="AL94" s="1"/>
+      <c r="AM94" s="1"/>
+      <c r="AN94" s="1"/>
+      <c r="AO94" s="1"/>
+      <c r="AP94" s="1"/>
+      <c r="AQ94" s="1"/>
+      <c r="AR94" s="1"/>
+      <c r="AS94" s="1"/>
+      <c r="AT94" s="1"/>
+      <c r="AU94" s="1"/>
+      <c r="AV94" s="1"/>
+      <c r="AW94" s="1"/>
+      <c r="AX94" s="1"/>
+      <c r="AY94" s="1"/>
+      <c r="AZ94" s="1"/>
+      <c r="BA94" s="1"/>
+      <c r="BB94" s="1"/>
+      <c r="BC94" s="1"/>
+      <c r="BD94" s="1"/>
+      <c r="BE94" s="1"/>
+      <c r="BF94" s="1"/>
+      <c r="BG94" s="1"/>
+      <c r="BH94" s="1"/>
+      <c r="BI94" s="1"/>
+      <c r="BJ94" s="1"/>
+      <c r="BK94" s="1"/>
+      <c r="BL94" s="1"/>
+      <c r="BM94" s="1"/>
+      <c r="BN94" s="1"/>
+      <c r="BO94" s="1"/>
+      <c r="BP94" s="1"/>
+      <c r="BQ94" s="1"/>
+      <c r="BR94" s="1"/>
+      <c r="BS94" s="1"/>
+      <c r="BT94" s="1"/>
+    </row>
+    <row r="95" spans="1:72">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="1"/>
+      <c r="H95" s="1"/>
+      <c r="I95" s="1"/>
+      <c r="J95" s="1"/>
+      <c r="K95" s="1"/>
+      <c r="L95" s="1"/>
+      <c r="M95" s="1"/>
+      <c r="N95" s="1"/>
+      <c r="O95" s="1"/>
+      <c r="P95" s="1"/>
+      <c r="Q95" s="1"/>
+      <c r="R95" s="1"/>
+      <c r="S95" s="1"/>
+      <c r="T95" s="1"/>
+      <c r="U95" s="1"/>
+      <c r="V95" s="1"/>
+      <c r="W95" s="1"/>
+      <c r="X95" s="1"/>
+      <c r="Y95" s="1"/>
+      <c r="Z95" s="1"/>
+      <c r="AA95" s="1"/>
+      <c r="AB95" s="1"/>
+      <c r="AC95" s="1"/>
+      <c r="AD95" s="1"/>
+      <c r="AE95" s="1"/>
+      <c r="AF95" s="1"/>
+      <c r="AG95" s="1"/>
+      <c r="AH95" s="1"/>
+      <c r="AI95" s="1"/>
+      <c r="AJ95" s="1"/>
+      <c r="AK95" s="1"/>
+      <c r="AL95" s="1"/>
+      <c r="AM95" s="1"/>
+      <c r="AN95" s="1"/>
+      <c r="AO95" s="1"/>
+      <c r="AP95" s="1"/>
+      <c r="AQ95" s="1"/>
+      <c r="AR95" s="1"/>
+      <c r="AS95" s="1"/>
+      <c r="AT95" s="1"/>
+      <c r="AU95" s="1"/>
+      <c r="AV95" s="1"/>
+      <c r="AW95" s="1"/>
+      <c r="AX95" s="1"/>
+      <c r="AY95" s="1"/>
+      <c r="AZ95" s="1"/>
+      <c r="BA95" s="1"/>
+      <c r="BB95" s="1"/>
+      <c r="BC95" s="1"/>
+      <c r="BD95" s="1"/>
+      <c r="BE95" s="1"/>
+      <c r="BF95" s="1"/>
+      <c r="BG95" s="1"/>
+      <c r="BH95" s="1"/>
+      <c r="BI95" s="1"/>
+      <c r="BJ95" s="1"/>
+      <c r="BK95" s="1"/>
+      <c r="BL95" s="1"/>
+      <c r="BM95" s="1"/>
+      <c r="BN95" s="1"/>
+      <c r="BO95" s="1"/>
+      <c r="BP95" s="1"/>
+      <c r="BQ95" s="1"/>
+      <c r="BR95" s="1"/>
+      <c r="BS95" s="1"/>
+      <c r="BT95" s="1"/>
+    </row>
+    <row r="96" spans="1:72">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
+      <c r="H96" s="1"/>
+      <c r="I96" s="1"/>
+      <c r="J96" s="1"/>
+      <c r="K96" s="1"/>
+      <c r="L96" s="1"/>
+      <c r="M96" s="1"/>
+      <c r="N96" s="1"/>
+      <c r="O96" s="1"/>
+      <c r="P96" s="1"/>
+      <c r="Q96" s="1"/>
+      <c r="R96" s="1"/>
+      <c r="S96" s="1"/>
+      <c r="T96" s="1"/>
+      <c r="U96" s="1"/>
+      <c r="V96" s="1"/>
+      <c r="W96" s="1"/>
+      <c r="X96" s="1"/>
+      <c r="Y96" s="1"/>
+      <c r="Z96" s="1"/>
+      <c r="AA96" s="1"/>
+      <c r="AB96" s="1"/>
+      <c r="AC96" s="1"/>
+      <c r="AD96" s="1"/>
+      <c r="AE96" s="1"/>
+      <c r="AF96" s="1"/>
+      <c r="AG96" s="1"/>
+      <c r="AH96" s="1"/>
+      <c r="AI96" s="1"/>
+      <c r="AJ96" s="1"/>
+      <c r="AK96" s="1"/>
+      <c r="AL96" s="1"/>
+      <c r="AM96" s="1"/>
+      <c r="AN96" s="1"/>
+      <c r="AO96" s="1"/>
+      <c r="AP96" s="1"/>
+      <c r="AQ96" s="1"/>
+      <c r="AR96" s="1"/>
+      <c r="AS96" s="1"/>
+      <c r="AT96" s="1"/>
+      <c r="AU96" s="1"/>
+      <c r="AV96" s="1"/>
+      <c r="AW96" s="1"/>
+      <c r="AX96" s="1"/>
+      <c r="AY96" s="1"/>
+      <c r="AZ96" s="1"/>
+      <c r="BA96" s="1"/>
+      <c r="BB96" s="1"/>
+      <c r="BC96" s="1"/>
+      <c r="BD96" s="1"/>
+      <c r="BE96" s="1"/>
+      <c r="BF96" s="1"/>
+      <c r="BG96" s="1"/>
+      <c r="BH96" s="1"/>
+      <c r="BI96" s="1"/>
+      <c r="BJ96" s="1"/>
+      <c r="BK96" s="1"/>
+      <c r="BL96" s="1"/>
+      <c r="BM96" s="1"/>
+      <c r="BN96" s="1"/>
+      <c r="BO96" s="1"/>
+      <c r="BP96" s="1"/>
+      <c r="BQ96" s="1"/>
+      <c r="BR96" s="1"/>
+      <c r="BS96" s="1"/>
+      <c r="BT96" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>